<commit_message>
Changing the forecast models for Kahraman
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,219 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>17.03.202518</t>
-  </si>
-  <si>
-    <t>17.03.202519</t>
-  </si>
-  <si>
-    <t>17.03.202520</t>
-  </si>
-  <si>
-    <t>17.03.202521</t>
-  </si>
-  <si>
-    <t>17.03.202522</t>
-  </si>
-  <si>
-    <t>17.03.202523</t>
-  </si>
-  <si>
-    <t>17.03.202524</t>
-  </si>
-  <si>
-    <t>18.03.20251</t>
-  </si>
-  <si>
-    <t>18.03.20252</t>
-  </si>
-  <si>
-    <t>18.03.20253</t>
-  </si>
-  <si>
-    <t>18.03.20254</t>
-  </si>
-  <si>
-    <t>18.03.20255</t>
-  </si>
-  <si>
-    <t>18.03.20256</t>
-  </si>
-  <si>
-    <t>18.03.20257</t>
-  </si>
-  <si>
-    <t>18.03.20258</t>
-  </si>
-  <si>
-    <t>18.03.20259</t>
-  </si>
-  <si>
-    <t>18.03.202510</t>
-  </si>
-  <si>
-    <t>18.03.202511</t>
-  </si>
-  <si>
-    <t>18.03.202512</t>
-  </si>
-  <si>
-    <t>18.03.202513</t>
-  </si>
-  <si>
-    <t>18.03.202514</t>
-  </si>
-  <si>
-    <t>18.03.202515</t>
-  </si>
-  <si>
-    <t>18.03.202516</t>
-  </si>
-  <si>
-    <t>18.03.202517</t>
-  </si>
-  <si>
-    <t>18.03.202518</t>
-  </si>
-  <si>
-    <t>18.03.202519</t>
-  </si>
-  <si>
-    <t>18.03.202520</t>
-  </si>
-  <si>
-    <t>18.03.202521</t>
-  </si>
-  <si>
-    <t>18.03.202522</t>
-  </si>
-  <si>
-    <t>18.03.202523</t>
-  </si>
-  <si>
-    <t>18.03.202524</t>
-  </si>
-  <si>
-    <t>19.03.20251</t>
-  </si>
-  <si>
-    <t>19.03.20252</t>
-  </si>
-  <si>
-    <t>19.03.20253</t>
-  </si>
-  <si>
-    <t>19.03.20254</t>
-  </si>
-  <si>
-    <t>19.03.20255</t>
-  </si>
-  <si>
-    <t>19.03.20256</t>
-  </si>
-  <si>
-    <t>19.03.20257</t>
-  </si>
-  <si>
-    <t>19.03.20258</t>
-  </si>
-  <si>
-    <t>19.03.20259</t>
-  </si>
-  <si>
-    <t>19.03.202510</t>
-  </si>
-  <si>
-    <t>19.03.202511</t>
-  </si>
-  <si>
-    <t>19.03.202512</t>
-  </si>
-  <si>
-    <t>19.03.202513</t>
-  </si>
-  <si>
-    <t>19.03.202514</t>
-  </si>
-  <si>
-    <t>19.03.202515</t>
-  </si>
-  <si>
-    <t>19.03.202516</t>
-  </si>
-  <si>
-    <t>19.03.202517</t>
-  </si>
-  <si>
-    <t>19.03.202518</t>
-  </si>
-  <si>
-    <t>19.03.202519</t>
-  </si>
-  <si>
-    <t>19.03.202520</t>
-  </si>
-  <si>
-    <t>19.03.202521</t>
-  </si>
-  <si>
-    <t>19.03.202522</t>
-  </si>
-  <si>
-    <t>19.03.202523</t>
-  </si>
-  <si>
-    <t>19.03.202524</t>
-  </si>
-  <si>
-    <t>20.03.20251</t>
-  </si>
-  <si>
-    <t>20.03.20252</t>
-  </si>
-  <si>
-    <t>20.03.20253</t>
-  </si>
-  <si>
-    <t>20.03.20254</t>
-  </si>
-  <si>
-    <t>20.03.20255</t>
-  </si>
-  <si>
-    <t>20.03.20256</t>
-  </si>
-  <si>
-    <t>20.03.20257</t>
-  </si>
-  <si>
-    <t>20.03.20258</t>
-  </si>
-  <si>
-    <t>20.03.20259</t>
-  </si>
-  <si>
-    <t>20.03.202510</t>
-  </si>
-  <si>
-    <t>20.03.202511</t>
-  </si>
-  <si>
-    <t>20.03.202512</t>
-  </si>
-  <si>
-    <t>20.03.202513</t>
-  </si>
-  <si>
-    <t>20.03.202514</t>
-  </si>
-  <si>
-    <t>20.03.202515</t>
-  </si>
-  <si>
-    <t>20.03.202516</t>
-  </si>
-  <si>
     <t>20.03.202517</t>
   </si>
   <si>
@@ -533,6 +320,219 @@
   </si>
   <si>
     <t>24.03.202518</t>
+  </si>
+  <si>
+    <t>24.03.202519</t>
+  </si>
+  <si>
+    <t>24.03.202520</t>
+  </si>
+  <si>
+    <t>24.03.202521</t>
+  </si>
+  <si>
+    <t>24.03.202522</t>
+  </si>
+  <si>
+    <t>24.03.202523</t>
+  </si>
+  <si>
+    <t>24.03.202524</t>
+  </si>
+  <si>
+    <t>25.03.20251</t>
+  </si>
+  <si>
+    <t>25.03.20252</t>
+  </si>
+  <si>
+    <t>25.03.20253</t>
+  </si>
+  <si>
+    <t>25.03.20254</t>
+  </si>
+  <si>
+    <t>25.03.20255</t>
+  </si>
+  <si>
+    <t>25.03.20256</t>
+  </si>
+  <si>
+    <t>25.03.20257</t>
+  </si>
+  <si>
+    <t>25.03.20258</t>
+  </si>
+  <si>
+    <t>25.03.20259</t>
+  </si>
+  <si>
+    <t>25.03.202510</t>
+  </si>
+  <si>
+    <t>25.03.202511</t>
+  </si>
+  <si>
+    <t>25.03.202512</t>
+  </si>
+  <si>
+    <t>25.03.202513</t>
+  </si>
+  <si>
+    <t>25.03.202514</t>
+  </si>
+  <si>
+    <t>25.03.202515</t>
+  </si>
+  <si>
+    <t>25.03.202516</t>
+  </si>
+  <si>
+    <t>25.03.202517</t>
+  </si>
+  <si>
+    <t>25.03.202518</t>
+  </si>
+  <si>
+    <t>25.03.202519</t>
+  </si>
+  <si>
+    <t>25.03.202520</t>
+  </si>
+  <si>
+    <t>25.03.202521</t>
+  </si>
+  <si>
+    <t>25.03.202522</t>
+  </si>
+  <si>
+    <t>25.03.202523</t>
+  </si>
+  <si>
+    <t>25.03.202524</t>
+  </si>
+  <si>
+    <t>26.03.20251</t>
+  </si>
+  <si>
+    <t>26.03.20252</t>
+  </si>
+  <si>
+    <t>26.03.20253</t>
+  </si>
+  <si>
+    <t>26.03.20254</t>
+  </si>
+  <si>
+    <t>26.03.20255</t>
+  </si>
+  <si>
+    <t>26.03.20256</t>
+  </si>
+  <si>
+    <t>26.03.20257</t>
+  </si>
+  <si>
+    <t>26.03.20258</t>
+  </si>
+  <si>
+    <t>26.03.20259</t>
+  </si>
+  <si>
+    <t>26.03.202510</t>
+  </si>
+  <si>
+    <t>26.03.202511</t>
+  </si>
+  <si>
+    <t>26.03.202512</t>
+  </si>
+  <si>
+    <t>26.03.202513</t>
+  </si>
+  <si>
+    <t>26.03.202514</t>
+  </si>
+  <si>
+    <t>26.03.202515</t>
+  </si>
+  <si>
+    <t>26.03.202516</t>
+  </si>
+  <si>
+    <t>26.03.202517</t>
+  </si>
+  <si>
+    <t>26.03.202518</t>
+  </si>
+  <si>
+    <t>26.03.202519</t>
+  </si>
+  <si>
+    <t>26.03.202520</t>
+  </si>
+  <si>
+    <t>26.03.202521</t>
+  </si>
+  <si>
+    <t>26.03.202522</t>
+  </si>
+  <si>
+    <t>26.03.202523</t>
+  </si>
+  <si>
+    <t>26.03.202524</t>
+  </si>
+  <si>
+    <t>27.03.20251</t>
+  </si>
+  <si>
+    <t>27.03.20252</t>
+  </si>
+  <si>
+    <t>27.03.20253</t>
+  </si>
+  <si>
+    <t>27.03.20254</t>
+  </si>
+  <si>
+    <t>27.03.20255</t>
+  </si>
+  <si>
+    <t>27.03.20256</t>
+  </si>
+  <si>
+    <t>27.03.20257</t>
+  </si>
+  <si>
+    <t>27.03.20258</t>
+  </si>
+  <si>
+    <t>27.03.20259</t>
+  </si>
+  <si>
+    <t>27.03.202510</t>
+  </si>
+  <si>
+    <t>27.03.202511</t>
+  </si>
+  <si>
+    <t>27.03.202512</t>
+  </si>
+  <si>
+    <t>27.03.202513</t>
+  </si>
+  <si>
+    <t>27.03.202514</t>
+  </si>
+  <si>
+    <t>27.03.202515</t>
+  </si>
+  <si>
+    <t>27.03.202516</t>
+  </si>
+  <si>
+    <t>27.03.202517</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>0.021</v>
+        <v>0.011</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.629</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.054</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45733</v>
+        <v>45736</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45734</v>
+        <v>45736</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>0.091</v>
+        <v>0.021</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>0.302</v>
+        <v>0.583</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>0.625</v>
+        <v>1.581</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B19">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>0.8129999999999999</v>
+        <v>2.647</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>0.915</v>
+        <v>3.366</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>1.379</v>
+        <v>3.95</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B22">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>1.369</v>
+        <v>4.181</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>1.354</v>
+        <v>4.156</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24">
-        <v>1.205</v>
+        <v>3.819</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B25">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>0.859</v>
+        <v>3.032</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B26">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>0.321</v>
+        <v>1.72</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B27">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27">
-        <v>0.018</v>
+        <v>0.662</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B28">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>0.054</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B30">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B31">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="B32">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45735</v>
+        <v>45737</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>0.547</v>
+        <v>0.013</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B41">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41">
-        <v>1.3</v>
+        <v>0.443</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42">
-        <v>2.273</v>
+        <v>1.451</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43">
-        <v>3.329</v>
+        <v>2.163</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B44">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>3.531</v>
+        <v>2.484</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B45">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>3.547</v>
+        <v>2.341</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B46">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>3.558</v>
+        <v>2.148</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B47">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>3.184</v>
+        <v>1.694</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B48">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>2.392</v>
+        <v>1.368</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B49">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>1.674</v>
+        <v>1.115</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B50">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50">
-        <v>0.644</v>
+        <v>0.77</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B51">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C51">
-        <v>0.029</v>
+        <v>0.205</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B52">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B53">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B54">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B55">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45735</v>
+        <v>45738</v>
       </c>
       <c r="B56">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B64">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>0.548</v>
+        <v>0.013</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65">
-        <v>1.426</v>
+        <v>0.195</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B66">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>2.283</v>
+        <v>0.766</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B67">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>3.29</v>
+        <v>1.282</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B68">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>3.491</v>
+        <v>1.513</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B69">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69">
-        <v>3.447</v>
+        <v>1.622</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B70">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C70">
-        <v>3.449</v>
+        <v>1.529</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B71">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71">
-        <v>3.2</v>
+        <v>1.41</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B72">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C72">
-        <v>2.408</v>
+        <v>1.114</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B73">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C73">
-        <v>1.674</v>
+        <v>0.842</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B74">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C74">
-        <v>0.641</v>
+        <v>0.596</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B75">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C75">
-        <v>0.033</v>
+        <v>0.132</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B76">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C76">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B77">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B78">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B79">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45736</v>
+        <v>45739</v>
       </c>
       <c r="B80">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B86">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B87">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B88">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>0.544</v>
+        <v>0.013</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B89">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C89">
-        <v>1.383</v>
+        <v>0.128</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B90">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C90">
-        <v>2.223</v>
+        <v>0.351</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B91">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C91">
-        <v>3.322</v>
+        <v>0.757</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B92">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C92">
-        <v>3.47</v>
+        <v>0.871</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B93">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>3.447</v>
+        <v>1.219</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B94">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C94">
-        <v>3.345</v>
+        <v>1.482</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B95">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C95">
-        <v>3.117</v>
+        <v>1.427</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B96">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C96">
-        <v>2.269</v>
+        <v>1.349</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B97">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C97">
-        <v>1.424</v>
+        <v>1.208</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B98">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C98">
-        <v>0.5620000000000001</v>
+        <v>0.783</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B99">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C99">
-        <v>0.033</v>
+        <v>0.252</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B100">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C100">
-        <v>0.013</v>
+        <v>0.023</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,10 +2302,10 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B101">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C101">
         <v>0.013</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B102">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B103">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="B104">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B109">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B110">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B111">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B112">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C112">
-        <v>0.319</v>
+        <v>0.022</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B113">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C113">
-        <v>1.248</v>
+        <v>0.45</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B114">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C114">
-        <v>2.005</v>
+        <v>1.376</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B115">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C115">
-        <v>2.567</v>
+        <v>2.179</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B116">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C116">
-        <v>3.006</v>
+        <v>2.918</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B117">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C117">
-        <v>3.114</v>
+        <v>3.113</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B118">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C118">
-        <v>2.931</v>
+        <v>3.154</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B119">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C119">
-        <v>2.295</v>
+        <v>3.055</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B120">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C120">
-        <v>1.772</v>
+        <v>2.49</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B121">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C121">
-        <v>1.132</v>
+        <v>1.52</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B122">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C122">
-        <v>0.326</v>
+        <v>0.783</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B123">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C123">
-        <v>0.023</v>
+        <v>0.2</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B124">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C124">
-        <v>0.013</v>
+        <v>0.017</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B125">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B126">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B127">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B128">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B131">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B132">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B133">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B134">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B135">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B136">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C136">
-        <v>0.178</v>
+        <v>0.013</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B137">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C137">
-        <v>0.607</v>
+        <v>0.247</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B138">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C138">
-        <v>1.05</v>
+        <v>0.922</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B139">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C139">
-        <v>1.366</v>
+        <v>1.752</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B140">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C140">
-        <v>1.834</v>
+        <v>2.607</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B141">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C141">
-        <v>2.141</v>
+        <v>3.153</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B142">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C142">
-        <v>2.246</v>
+        <v>3.349</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B143">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C143">
-        <v>1.998</v>
+        <v>3.327</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B144">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C144">
-        <v>1.28</v>
+        <v>3.014</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B145">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C145">
-        <v>0.826</v>
+        <v>2.272</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B146">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C146">
-        <v>0.202</v>
+        <v>1.427</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B147">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C147">
-        <v>0.017</v>
+        <v>0.439</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B148">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B149">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B150">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B151">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B152">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B154">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B155">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B156">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B157">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B158">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B159">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B160">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C160">
-        <v>0.19</v>
+        <v>0.014</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B161">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C161">
-        <v>0.735</v>
+        <v>0.116</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B162">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C162">
-        <v>1.133</v>
+        <v>0.312</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B163">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C163">
-        <v>1.362</v>
+        <v>0.639</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B164">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C164">
-        <v>1.424</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B165">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C165">
-        <v>1.955</v>
+        <v>0.996</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B166">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C166">
-        <v>2.1</v>
+        <v>1.02</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B167">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C167">
-        <v>1.791</v>
+        <v>0.971</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B168">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C168">
-        <v>1.312</v>
+        <v>0.801</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B169">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C169">
-        <v>0.763</v>
+        <v>0.734</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B170">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C170">
-        <v>0.198</v>
+        <v>0.369</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Remmoving past portfolio data
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,120 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>20.03.202517</t>
-  </si>
-  <si>
-    <t>20.03.202518</t>
-  </si>
-  <si>
-    <t>20.03.202519</t>
-  </si>
-  <si>
-    <t>20.03.202520</t>
-  </si>
-  <si>
-    <t>20.03.202521</t>
-  </si>
-  <si>
-    <t>20.03.202522</t>
-  </si>
-  <si>
-    <t>20.03.202523</t>
-  </si>
-  <si>
-    <t>20.03.202524</t>
-  </si>
-  <si>
-    <t>21.03.20251</t>
-  </si>
-  <si>
-    <t>21.03.20252</t>
-  </si>
-  <si>
-    <t>21.03.20253</t>
-  </si>
-  <si>
-    <t>21.03.20254</t>
-  </si>
-  <si>
-    <t>21.03.20255</t>
-  </si>
-  <si>
-    <t>21.03.20256</t>
-  </si>
-  <si>
-    <t>21.03.20257</t>
-  </si>
-  <si>
-    <t>21.03.20258</t>
-  </si>
-  <si>
-    <t>21.03.20259</t>
-  </si>
-  <si>
-    <t>21.03.202510</t>
-  </si>
-  <si>
-    <t>21.03.202511</t>
-  </si>
-  <si>
-    <t>21.03.202512</t>
-  </si>
-  <si>
-    <t>21.03.202513</t>
-  </si>
-  <si>
-    <t>21.03.202514</t>
-  </si>
-  <si>
-    <t>21.03.202515</t>
-  </si>
-  <si>
-    <t>21.03.202516</t>
-  </si>
-  <si>
-    <t>21.03.202517</t>
-  </si>
-  <si>
-    <t>21.03.202518</t>
-  </si>
-  <si>
-    <t>21.03.202519</t>
-  </si>
-  <si>
-    <t>21.03.202520</t>
-  </si>
-  <si>
-    <t>21.03.202521</t>
-  </si>
-  <si>
-    <t>21.03.202522</t>
-  </si>
-  <si>
-    <t>21.03.202523</t>
-  </si>
-  <si>
-    <t>21.03.202524</t>
-  </si>
-  <si>
-    <t>22.03.20251</t>
-  </si>
-  <si>
-    <t>22.03.20252</t>
-  </si>
-  <si>
-    <t>22.03.20253</t>
-  </si>
-  <si>
-    <t>22.03.20254</t>
-  </si>
-  <si>
-    <t>22.03.20255</t>
-  </si>
-  <si>
-    <t>22.03.20256</t>
-  </si>
-  <si>
     <t>22.03.20257</t>
   </si>
   <si>
@@ -533,6 +419,120 @@
   </si>
   <si>
     <t>27.03.202517</t>
+  </si>
+  <si>
+    <t>27.03.202518</t>
+  </si>
+  <si>
+    <t>27.03.202519</t>
+  </si>
+  <si>
+    <t>27.03.202520</t>
+  </si>
+  <si>
+    <t>27.03.202521</t>
+  </si>
+  <si>
+    <t>27.03.202522</t>
+  </si>
+  <si>
+    <t>27.03.202523</t>
+  </si>
+  <si>
+    <t>27.03.202524</t>
+  </si>
+  <si>
+    <t>28.03.20251</t>
+  </si>
+  <si>
+    <t>28.03.20252</t>
+  </si>
+  <si>
+    <t>28.03.20253</t>
+  </si>
+  <si>
+    <t>28.03.20254</t>
+  </si>
+  <si>
+    <t>28.03.20255</t>
+  </si>
+  <si>
+    <t>28.03.20256</t>
+  </si>
+  <si>
+    <t>28.03.20257</t>
+  </si>
+  <si>
+    <t>28.03.20258</t>
+  </si>
+  <si>
+    <t>28.03.20259</t>
+  </si>
+  <si>
+    <t>28.03.202510</t>
+  </si>
+  <si>
+    <t>28.03.202511</t>
+  </si>
+  <si>
+    <t>28.03.202512</t>
+  </si>
+  <si>
+    <t>28.03.202513</t>
+  </si>
+  <si>
+    <t>28.03.202514</t>
+  </si>
+  <si>
+    <t>28.03.202515</t>
+  </si>
+  <si>
+    <t>28.03.202516</t>
+  </si>
+  <si>
+    <t>28.03.202517</t>
+  </si>
+  <si>
+    <t>28.03.202518</t>
+  </si>
+  <si>
+    <t>28.03.202519</t>
+  </si>
+  <si>
+    <t>28.03.202520</t>
+  </si>
+  <si>
+    <t>28.03.202521</t>
+  </si>
+  <si>
+    <t>28.03.202522</t>
+  </si>
+  <si>
+    <t>28.03.202523</t>
+  </si>
+  <si>
+    <t>28.03.202524</t>
+  </si>
+  <si>
+    <t>29.03.20251</t>
+  </si>
+  <si>
+    <t>29.03.20252</t>
+  </si>
+  <si>
+    <t>29.03.20253</t>
+  </si>
+  <si>
+    <t>29.03.20254</t>
+  </si>
+  <si>
+    <t>29.03.20255</t>
+  </si>
+  <si>
+    <t>29.03.20256</t>
+  </si>
+  <si>
+    <t>29.03.20257</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0.011</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>0.629</v>
+        <v>0.332</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>0.054</v>
+        <v>0.779</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>0.011</v>
+        <v>1.261</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>0.011</v>
+        <v>1.463</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>0.011</v>
+        <v>1.51</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>0.011</v>
+        <v>1.403</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>0.011</v>
+        <v>1.37</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>0.011</v>
+        <v>1.162</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>0.011</v>
+        <v>1.058</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>0.011</v>
+        <v>0.672</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>0.011</v>
+        <v>0.196</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>0.021</v>
+        <v>0.013</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>0.583</v>
+        <v>0.013</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>1.581</v>
+        <v>0.013</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>2.647</v>
+        <v>0.013</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>3.366</v>
+        <v>0.013</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>3.95</v>
+        <v>0.012</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>4.181</v>
+        <v>0.012</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B23">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>4.156</v>
+        <v>0.012</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>3.819</v>
+        <v>0.012</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>3.032</v>
+        <v>0.012</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B26">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>1.72</v>
+        <v>0.013</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>0.662</v>
+        <v>0.2</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>0.054</v>
+        <v>0.774</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>0.011</v>
+        <v>1.473</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B30">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C30">
-        <v>0.011</v>
+        <v>1.599</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B31">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C31">
-        <v>0.011</v>
+        <v>1.647</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B32">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C32">
-        <v>0.011</v>
+        <v>1.464</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45737</v>
+        <v>45739</v>
       </c>
       <c r="B33">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C33">
-        <v>0.011</v>
+        <v>1.399</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C34">
-        <v>0.011</v>
+        <v>1.043</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C35">
-        <v>0.011</v>
+        <v>0.798</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C36">
-        <v>0.011</v>
+        <v>0.62</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C37">
-        <v>0.012</v>
+        <v>0.196</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C38">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C39">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C40">
         <v>0.013</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C41">
-        <v>0.443</v>
+        <v>0.013</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C42">
-        <v>1.451</v>
+        <v>0.012</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45738</v>
+        <v>45739</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C43">
-        <v>2.163</v>
+        <v>0.012</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>2.484</v>
+        <v>0.013</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>2.341</v>
+        <v>0.012</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B46">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>2.148</v>
+        <v>0.012</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>1.694</v>
+        <v>0.013</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B48">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>1.368</v>
+        <v>0.013</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B49">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>1.115</v>
+        <v>0.013</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B50">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C50">
-        <v>0.77</v>
+        <v>0.013</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C51">
-        <v>0.205</v>
+        <v>0.132</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B52">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C52">
-        <v>0.014</v>
+        <v>0.578</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B53">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>0.013</v>
+        <v>0.858</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B54">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C54">
-        <v>0.013</v>
+        <v>1.258</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>0.013</v>
+        <v>1.436</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B56">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C56">
-        <v>0.013</v>
+        <v>1.352</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C57">
-        <v>0.013</v>
+        <v>1.3</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C58">
-        <v>0.013</v>
+        <v>1.165</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C59">
-        <v>0.013</v>
+        <v>0.975</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C60">
-        <v>0.013</v>
+        <v>0.761</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C61">
-        <v>0.012</v>
+        <v>0.198</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C62">
-        <v>0.012</v>
+        <v>0.022</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C63">
         <v>0.012</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C64">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C65">
-        <v>0.195</v>
+        <v>0.012</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C66">
-        <v>0.766</v>
+        <v>0.012</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45739</v>
+        <v>45740</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C67">
-        <v>1.282</v>
+        <v>0.012</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>1.513</v>
+        <v>0.012</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B69">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C69">
-        <v>1.622</v>
+        <v>0.012</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B70">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C70">
-        <v>1.529</v>
+        <v>0.012</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>1.41</v>
+        <v>0.012</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C72">
-        <v>1.114</v>
+        <v>0.012</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B73">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>0.842</v>
+        <v>0.012</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B74">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C74">
-        <v>0.596</v>
+        <v>0.013</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C75">
-        <v>0.132</v>
+        <v>0.245</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B76">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C76">
-        <v>0.014</v>
+        <v>0.77</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B77">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>0.013</v>
+        <v>1.632</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B78">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C78">
-        <v>0.013</v>
+        <v>2.691</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B79">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C79">
-        <v>0.013</v>
+        <v>3.408</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B80">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C80">
-        <v>0.013</v>
+        <v>3.75</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45739</v>
+        <v>45741</v>
       </c>
       <c r="B81">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C81">
-        <v>0.013</v>
+        <v>3.662</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C82">
-        <v>0.013</v>
+        <v>3.11</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C83">
-        <v>0.013</v>
+        <v>2.217</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C84">
-        <v>0.013</v>
+        <v>1.426</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C85">
-        <v>0.013</v>
+        <v>0.445</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C86">
-        <v>0.013</v>
+        <v>0.037</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B87">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C87">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B88">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C88">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C89">
-        <v>0.128</v>
+        <v>0.012</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C90">
-        <v>0.351</v>
+        <v>0.013</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="B91">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C91">
-        <v>0.757</v>
+        <v>0.013</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B92">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C92">
-        <v>0.871</v>
+        <v>0.013</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B93">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C93">
-        <v>1.219</v>
+        <v>0.013</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C94">
-        <v>1.482</v>
+        <v>0.013</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B95">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C95">
-        <v>1.427</v>
+        <v>0.013</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C96">
-        <v>1.349</v>
+        <v>0.013</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B97">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>1.208</v>
+        <v>0.013</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B98">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C98">
-        <v>0.783</v>
+        <v>0.013</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B99">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C99">
-        <v>0.252</v>
+        <v>0.128</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B100">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C100">
-        <v>0.023</v>
+        <v>0.351</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C101">
-        <v>0.013</v>
+        <v>0.766</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B102">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C102">
-        <v>0.013</v>
+        <v>1.043</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B103">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C103">
-        <v>0.013</v>
+        <v>1.334</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B104">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C104">
-        <v>0.013</v>
+        <v>1.345</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="B105">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C105">
-        <v>0.013</v>
+        <v>1.179</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C106">
-        <v>0.012</v>
+        <v>0.857</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C107">
-        <v>0.012</v>
+        <v>0.841</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C108">
-        <v>0.012</v>
+        <v>0.739</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B109">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C109">
-        <v>0.012</v>
+        <v>0.2</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C110">
-        <v>0.012</v>
+        <v>0.023</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B111">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C111">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B112">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C112">
-        <v>0.022</v>
+        <v>0.013</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C113">
-        <v>0.45</v>
+        <v>0.013</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B114">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C114">
-        <v>1.376</v>
+        <v>0.013</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C115">
-        <v>2.179</v>
+        <v>0.013</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B116">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C116">
-        <v>2.918</v>
+        <v>0.013</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B117">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C117">
-        <v>3.113</v>
+        <v>0.013</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B118">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C118">
-        <v>3.154</v>
+        <v>0.013</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B119">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C119">
-        <v>3.055</v>
+        <v>0.013</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B120">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C120">
-        <v>2.49</v>
+        <v>0.013</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B121">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C121">
-        <v>1.52</v>
+        <v>0.013</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B122">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C122">
-        <v>0.783</v>
+        <v>0.013</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B123">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C123">
-        <v>0.2</v>
+        <v>0.056</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B124">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C124">
-        <v>0.017</v>
+        <v>0.202</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B125">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C125">
-        <v>0.013</v>
+        <v>0.317</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B126">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C126">
-        <v>0.013</v>
+        <v>0.38</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B127">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C127">
-        <v>0.013</v>
+        <v>0.641</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B128">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C128">
-        <v>0.013</v>
+        <v>0.76</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="B129">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C129">
-        <v>0.013</v>
+        <v>0.794</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C130">
-        <v>0.013</v>
+        <v>0.751</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C131">
-        <v>0.013</v>
+        <v>0.607</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B132">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C132">
-        <v>0.013</v>
+        <v>0.327</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C133">
-        <v>0.013</v>
+        <v>0.128</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B134">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C134">
-        <v>0.012</v>
+        <v>0.015</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C135">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B136">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C136">
         <v>0.013</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B137">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C137">
-        <v>0.247</v>
+        <v>0.013</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C138">
-        <v>0.922</v>
+        <v>0.013</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B139">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C139">
-        <v>1.752</v>
+        <v>0.013</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C140">
-        <v>2.607</v>
+        <v>0.013</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B141">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C141">
-        <v>3.153</v>
+        <v>0.013</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B142">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C142">
-        <v>3.349</v>
+        <v>0.013</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B143">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C143">
-        <v>3.327</v>
+        <v>0.013</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B144">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C144">
-        <v>3.014</v>
+        <v>0.013</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B145">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C145">
-        <v>2.272</v>
+        <v>0.013</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B146">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C146">
-        <v>1.427</v>
+        <v>0.015</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B147">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C147">
-        <v>0.439</v>
+        <v>0.128</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B148">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C148">
-        <v>0.037</v>
+        <v>0.312</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B149">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C149">
-        <v>0.012</v>
+        <v>0.594</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B150">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C150">
-        <v>0.012</v>
+        <v>0.621</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B151">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C151">
-        <v>0.012</v>
+        <v>0.641</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B152">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C152">
-        <v>0.012</v>
+        <v>0.621</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="B153">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C153">
-        <v>0.012</v>
+        <v>0.59</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C154">
-        <v>0.012</v>
+        <v>0.471</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C155">
-        <v>0.012</v>
+        <v>0.364</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B156">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C156">
-        <v>0.013</v>
+        <v>0.265</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B157">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C157">
-        <v>0.013</v>
+        <v>0.128</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B158">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C158">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B159">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C159">
         <v>0.013</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C160">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B161">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C161">
-        <v>0.116</v>
+        <v>0.013</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B162">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C162">
-        <v>0.312</v>
+        <v>0.013</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B163">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C163">
-        <v>0.639</v>
+        <v>0.013</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B164">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C164">
-        <v>0.8080000000000001</v>
+        <v>0.012</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B165">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C165">
-        <v>0.996</v>
+        <v>0.012</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C166">
-        <v>1.02</v>
+        <v>0.012</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B167">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C167">
-        <v>0.971</v>
+        <v>0.012</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B168">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C168">
-        <v>0.801</v>
+        <v>0.012</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B169">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C169">
-        <v>0.734</v>
+        <v>0.012</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45743</v>
+        <v>45745</v>
       </c>
       <c r="B170">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C170">
-        <v>0.369</v>
+        <v>0.031</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Replacing the models for Kahraman with better ones
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,237 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>22.03.20257</t>
-  </si>
-  <si>
-    <t>22.03.20258</t>
-  </si>
-  <si>
-    <t>22.03.20259</t>
-  </si>
-  <si>
-    <t>22.03.202510</t>
-  </si>
-  <si>
-    <t>22.03.202511</t>
-  </si>
-  <si>
-    <t>22.03.202512</t>
-  </si>
-  <si>
-    <t>22.03.202513</t>
-  </si>
-  <si>
-    <t>22.03.202514</t>
-  </si>
-  <si>
-    <t>22.03.202515</t>
-  </si>
-  <si>
-    <t>22.03.202516</t>
-  </si>
-  <si>
-    <t>22.03.202517</t>
-  </si>
-  <si>
-    <t>22.03.202518</t>
-  </si>
-  <si>
-    <t>22.03.202519</t>
-  </si>
-  <si>
-    <t>22.03.202520</t>
-  </si>
-  <si>
-    <t>22.03.202521</t>
-  </si>
-  <si>
-    <t>22.03.202522</t>
-  </si>
-  <si>
-    <t>22.03.202523</t>
-  </si>
-  <si>
-    <t>22.03.202524</t>
-  </si>
-  <si>
-    <t>23.03.20251</t>
-  </si>
-  <si>
-    <t>23.03.20252</t>
-  </si>
-  <si>
-    <t>23.03.20253</t>
-  </si>
-  <si>
-    <t>23.03.20254</t>
-  </si>
-  <si>
-    <t>23.03.20255</t>
-  </si>
-  <si>
-    <t>23.03.20256</t>
-  </si>
-  <si>
-    <t>23.03.20257</t>
-  </si>
-  <si>
-    <t>23.03.20258</t>
-  </si>
-  <si>
-    <t>23.03.20259</t>
-  </si>
-  <si>
-    <t>23.03.202510</t>
-  </si>
-  <si>
-    <t>23.03.202511</t>
-  </si>
-  <si>
-    <t>23.03.202512</t>
-  </si>
-  <si>
-    <t>23.03.202513</t>
-  </si>
-  <si>
-    <t>23.03.202514</t>
-  </si>
-  <si>
-    <t>23.03.202515</t>
-  </si>
-  <si>
-    <t>23.03.202516</t>
-  </si>
-  <si>
-    <t>23.03.202517</t>
-  </si>
-  <si>
-    <t>23.03.202518</t>
-  </si>
-  <si>
-    <t>23.03.202519</t>
-  </si>
-  <si>
-    <t>23.03.202520</t>
-  </si>
-  <si>
-    <t>23.03.202521</t>
-  </si>
-  <si>
-    <t>23.03.202522</t>
-  </si>
-  <si>
-    <t>23.03.202523</t>
-  </si>
-  <si>
-    <t>23.03.202524</t>
-  </si>
-  <si>
-    <t>24.03.20251</t>
-  </si>
-  <si>
-    <t>24.03.20252</t>
-  </si>
-  <si>
-    <t>24.03.20253</t>
-  </si>
-  <si>
-    <t>24.03.20254</t>
-  </si>
-  <si>
-    <t>24.03.20255</t>
-  </si>
-  <si>
-    <t>24.03.20256</t>
-  </si>
-  <si>
-    <t>24.03.20257</t>
-  </si>
-  <si>
-    <t>24.03.20258</t>
-  </si>
-  <si>
-    <t>24.03.20259</t>
-  </si>
-  <si>
-    <t>24.03.202510</t>
-  </si>
-  <si>
-    <t>24.03.202511</t>
-  </si>
-  <si>
-    <t>24.03.202512</t>
-  </si>
-  <si>
-    <t>24.03.202513</t>
-  </si>
-  <si>
-    <t>24.03.202514</t>
-  </si>
-  <si>
-    <t>24.03.202515</t>
-  </si>
-  <si>
-    <t>24.03.202516</t>
-  </si>
-  <si>
-    <t>24.03.202517</t>
-  </si>
-  <si>
-    <t>24.03.202518</t>
-  </si>
-  <si>
-    <t>24.03.202519</t>
-  </si>
-  <si>
-    <t>24.03.202520</t>
-  </si>
-  <si>
-    <t>24.03.202521</t>
-  </si>
-  <si>
-    <t>24.03.202522</t>
-  </si>
-  <si>
-    <t>24.03.202523</t>
-  </si>
-  <si>
-    <t>24.03.202524</t>
-  </si>
-  <si>
-    <t>25.03.20251</t>
-  </si>
-  <si>
-    <t>25.03.20252</t>
-  </si>
-  <si>
-    <t>25.03.20253</t>
-  </si>
-  <si>
-    <t>25.03.20254</t>
-  </si>
-  <si>
-    <t>25.03.20255</t>
-  </si>
-  <si>
-    <t>25.03.20256</t>
-  </si>
-  <si>
-    <t>25.03.20257</t>
-  </si>
-  <si>
-    <t>25.03.20258</t>
-  </si>
-  <si>
-    <t>25.03.20259</t>
-  </si>
-  <si>
-    <t>25.03.202510</t>
-  </si>
-  <si>
-    <t>25.03.202511</t>
-  </si>
-  <si>
     <t>25.03.202512</t>
   </si>
   <si>
@@ -533,6 +302,237 @@
   </si>
   <si>
     <t>29.03.20257</t>
+  </si>
+  <si>
+    <t>29.03.20258</t>
+  </si>
+  <si>
+    <t>29.03.20259</t>
+  </si>
+  <si>
+    <t>29.03.202510</t>
+  </si>
+  <si>
+    <t>29.03.202511</t>
+  </si>
+  <si>
+    <t>29.03.202512</t>
+  </si>
+  <si>
+    <t>29.03.202513</t>
+  </si>
+  <si>
+    <t>29.03.202514</t>
+  </si>
+  <si>
+    <t>29.03.202515</t>
+  </si>
+  <si>
+    <t>29.03.202516</t>
+  </si>
+  <si>
+    <t>29.03.202517</t>
+  </si>
+  <si>
+    <t>29.03.202518</t>
+  </si>
+  <si>
+    <t>29.03.202519</t>
+  </si>
+  <si>
+    <t>29.03.202520</t>
+  </si>
+  <si>
+    <t>29.03.202521</t>
+  </si>
+  <si>
+    <t>29.03.202522</t>
+  </si>
+  <si>
+    <t>29.03.202523</t>
+  </si>
+  <si>
+    <t>29.03.202524</t>
+  </si>
+  <si>
+    <t>30.03.20251</t>
+  </si>
+  <si>
+    <t>30.03.20252</t>
+  </si>
+  <si>
+    <t>30.03.20253</t>
+  </si>
+  <si>
+    <t>30.03.20254</t>
+  </si>
+  <si>
+    <t>30.03.20255</t>
+  </si>
+  <si>
+    <t>30.03.20256</t>
+  </si>
+  <si>
+    <t>30.03.20257</t>
+  </si>
+  <si>
+    <t>30.03.20258</t>
+  </si>
+  <si>
+    <t>30.03.20259</t>
+  </si>
+  <si>
+    <t>30.03.202510</t>
+  </si>
+  <si>
+    <t>30.03.202511</t>
+  </si>
+  <si>
+    <t>30.03.202512</t>
+  </si>
+  <si>
+    <t>30.03.202513</t>
+  </si>
+  <si>
+    <t>30.03.202514</t>
+  </si>
+  <si>
+    <t>30.03.202515</t>
+  </si>
+  <si>
+    <t>30.03.202516</t>
+  </si>
+  <si>
+    <t>30.03.202517</t>
+  </si>
+  <si>
+    <t>30.03.202518</t>
+  </si>
+  <si>
+    <t>30.03.202519</t>
+  </si>
+  <si>
+    <t>30.03.202520</t>
+  </si>
+  <si>
+    <t>30.03.202521</t>
+  </si>
+  <si>
+    <t>30.03.202522</t>
+  </si>
+  <si>
+    <t>30.03.202523</t>
+  </si>
+  <si>
+    <t>30.03.202524</t>
+  </si>
+  <si>
+    <t>31.03.20251</t>
+  </si>
+  <si>
+    <t>31.03.20252</t>
+  </si>
+  <si>
+    <t>31.03.20253</t>
+  </si>
+  <si>
+    <t>31.03.20254</t>
+  </si>
+  <si>
+    <t>31.03.20255</t>
+  </si>
+  <si>
+    <t>31.03.20256</t>
+  </si>
+  <si>
+    <t>31.03.20257</t>
+  </si>
+  <si>
+    <t>31.03.20258</t>
+  </si>
+  <si>
+    <t>31.03.20259</t>
+  </si>
+  <si>
+    <t>31.03.202510</t>
+  </si>
+  <si>
+    <t>31.03.202511</t>
+  </si>
+  <si>
+    <t>31.03.202512</t>
+  </si>
+  <si>
+    <t>31.03.202513</t>
+  </si>
+  <si>
+    <t>31.03.202514</t>
+  </si>
+  <si>
+    <t>31.03.202515</t>
+  </si>
+  <si>
+    <t>31.03.202516</t>
+  </si>
+  <si>
+    <t>31.03.202517</t>
+  </si>
+  <si>
+    <t>31.03.202518</t>
+  </si>
+  <si>
+    <t>31.03.202519</t>
+  </si>
+  <si>
+    <t>31.03.202520</t>
+  </si>
+  <si>
+    <t>31.03.202521</t>
+  </si>
+  <si>
+    <t>31.03.202522</t>
+  </si>
+  <si>
+    <t>31.03.202523</t>
+  </si>
+  <si>
+    <t>31.03.202524</t>
+  </si>
+  <si>
+    <t>01.04.20251</t>
+  </si>
+  <si>
+    <t>01.04.20252</t>
+  </si>
+  <si>
+    <t>01.04.20253</t>
+  </si>
+  <si>
+    <t>01.04.20254</t>
+  </si>
+  <si>
+    <t>01.04.20255</t>
+  </si>
+  <si>
+    <t>01.04.20256</t>
+  </si>
+  <si>
+    <t>01.04.20257</t>
+  </si>
+  <si>
+    <t>01.04.20258</t>
+  </si>
+  <si>
+    <t>01.04.20259</t>
+  </si>
+  <si>
+    <t>01.04.202510</t>
+  </si>
+  <si>
+    <t>01.04.202511</t>
+  </si>
+  <si>
+    <t>01.04.202512</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0.011</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>0.332</v>
+        <v>3.399</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>0.779</v>
+        <v>2.446</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>1.261</v>
+        <v>1.939</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>1.463</v>
+        <v>1.924</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>1.51</v>
+        <v>1.393</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>1.403</v>
+        <v>0.547</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>1.37</v>
+        <v>0.041</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1.162</v>
+        <v>0.012</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>1.058</v>
+        <v>0.012</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B12">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>0.672</v>
+        <v>0.012</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B13">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>0.196</v>
+        <v>0.012</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45738</v>
+        <v>45741</v>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45738</v>
+        <v>45742</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45738</v>
+        <v>45742</v>
       </c>
       <c r="B16">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45738</v>
+        <v>45742</v>
       </c>
       <c r="B17">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45738</v>
+        <v>45742</v>
       </c>
       <c r="B18">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45738</v>
+        <v>45742</v>
       </c>
       <c r="B19">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>0.012</v>
+        <v>0.022</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>0.012</v>
+        <v>0.301</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>0.012</v>
+        <v>0.793</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>0.012</v>
+        <v>1.249</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>0.012</v>
+        <v>1.381</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>0.013</v>
+        <v>1.408</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>0.2</v>
+        <v>1.427</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>0.774</v>
+        <v>1.388</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>1.473</v>
+        <v>0.999</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B30">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>1.599</v>
+        <v>0.76</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>1.647</v>
+        <v>0.346</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B32">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>1.464</v>
+        <v>0.128</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B33">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>1.399</v>
+        <v>0.015</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B34">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>1.043</v>
+        <v>0.013</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>0.798</v>
+        <v>0.013</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B36">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C36">
-        <v>0.62</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B37">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C37">
-        <v>0.196</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45739</v>
+        <v>45742</v>
       </c>
       <c r="B38">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C38">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45739</v>
+        <v>45743</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0.013</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45739</v>
+        <v>45743</v>
       </c>
       <c r="B40">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0.013</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45739</v>
+        <v>45743</v>
       </c>
       <c r="B41">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0.013</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45739</v>
+        <v>45743</v>
       </c>
       <c r="B42">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45739</v>
+        <v>45743</v>
       </c>
       <c r="B43">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C43">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C44">
         <v>0.013</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>0.012</v>
+        <v>0.061</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>0.013</v>
+        <v>0.204</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>0.013</v>
+        <v>0.334</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>0.013</v>
+        <v>0.621</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>0.013</v>
+        <v>0.798</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B51">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>0.132</v>
+        <v>0.805</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B52">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>0.578</v>
+        <v>0.801</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B53">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>0.858</v>
+        <v>0.737</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B54">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>1.258</v>
+        <v>0.637</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B55">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>1.436</v>
+        <v>0.368</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B56">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C56">
-        <v>1.352</v>
+        <v>0.128</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B57">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>1.3</v>
+        <v>0.014</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B58">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C58">
-        <v>1.165</v>
+        <v>0.013</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B59">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>0.975</v>
+        <v>0.013</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B60">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>0.761</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B61">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>0.198</v>
+        <v>0.013</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="B62">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C62">
-        <v>0.022</v>
+        <v>0.013</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="B63">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C63">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="B64">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C64">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="B65">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="B66">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C66">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="B67">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>0.012</v>
+        <v>0.015</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>0.012</v>
+        <v>0.091</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>0.012</v>
+        <v>0.207</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>0.012</v>
+        <v>0.357</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>0.012</v>
+        <v>0.618</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B74">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>0.013</v>
+        <v>0.704</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B75">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>0.245</v>
+        <v>0.753</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B76">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>0.77</v>
+        <v>0.749</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B77">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>1.632</v>
+        <v>0.743</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B78">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>2.691</v>
+        <v>0.745</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B79">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>3.408</v>
+        <v>0.598</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B80">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>3.75</v>
+        <v>0.196</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B81">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C81">
-        <v>3.662</v>
+        <v>0.023</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B82">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>3.11</v>
+        <v>0.013</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B83">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>2.217</v>
+        <v>0.013</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B84">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C84">
-        <v>1.426</v>
+        <v>0.013</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B85">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C85">
-        <v>0.445</v>
+        <v>0.013</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B86">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C86">
-        <v>0.037</v>
+        <v>0.013</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B87">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C87">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B88">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C88">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B89">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C89">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B90">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>0.013</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B91">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C91">
         <v>0.013</v>
@@ -2176,10 +2176,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C92">
         <v>0.013</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B94">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>0.013</v>
+        <v>0.12</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B95">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C95">
-        <v>0.013</v>
+        <v>0.259</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B96">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C96">
-        <v>0.013</v>
+        <v>0.545</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B97">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C97">
-        <v>0.013</v>
+        <v>0.776</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B98">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C98">
-        <v>0.013</v>
+        <v>0.863</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B99">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C99">
-        <v>0.128</v>
+        <v>0.983</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B100">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C100">
-        <v>0.351</v>
+        <v>1.044</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B101">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C101">
-        <v>0.766</v>
+        <v>0.993</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B102">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <v>1.043</v>
+        <v>0.992</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B103">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C103">
-        <v>1.334</v>
+        <v>0.781</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B104">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <v>1.345</v>
+        <v>0.274</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B105">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C105">
-        <v>1.179</v>
+        <v>0.038</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B106">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C106">
-        <v>0.857</v>
+        <v>0.013</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B107">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C107">
-        <v>0.841</v>
+        <v>0.013</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B108">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C108">
-        <v>0.739</v>
+        <v>0.013</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B109">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>0.2</v>
+        <v>0.013</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B110">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C110">
-        <v>0.023</v>
+        <v>0.013</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B111">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>0.013</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B112">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C112">
         <v>0.013</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B113">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C113">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B114">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C114">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B115">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C115">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C116">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C117">
-        <v>0.013</v>
+        <v>0.031</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C118">
-        <v>0.013</v>
+        <v>0.305</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B119">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C119">
-        <v>0.013</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B120">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C120">
-        <v>0.013</v>
+        <v>1.582</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B121">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C121">
-        <v>0.013</v>
+        <v>1.791</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B122">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C122">
-        <v>0.013</v>
+        <v>2.046</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B123">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C123">
-        <v>0.056</v>
+        <v>2.335</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B124">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C124">
-        <v>0.202</v>
+        <v>2.335</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B125">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C125">
-        <v>0.317</v>
+        <v>1.95</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B126">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C126">
-        <v>0.38</v>
+        <v>1.511</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B127">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C127">
-        <v>0.641</v>
+        <v>0.948</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B128">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C128">
-        <v>0.76</v>
+        <v>0.3</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B129">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C129">
-        <v>0.794</v>
+        <v>0.041</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B130">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C130">
-        <v>0.751</v>
+        <v>0.012</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B131">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C131">
-        <v>0.607</v>
+        <v>0.012</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B132">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C132">
-        <v>0.327</v>
+        <v>0.012</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B133">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C133">
-        <v>0.128</v>
+        <v>0.012</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B134">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C134">
-        <v>0.015</v>
+        <v>0.012</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B135">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C135">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B136">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C136">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B137">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C137">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B138">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C138">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B139">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C139">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B141">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>0.013</v>
+        <v>0.022</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B142">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>0.013</v>
+        <v>0.202</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B143">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C143">
-        <v>0.013</v>
+        <v>0.625</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B144">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C144">
-        <v>0.013</v>
+        <v>0.996</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B145">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C145">
-        <v>0.013</v>
+        <v>1.452</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B146">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C146">
-        <v>0.015</v>
+        <v>1.605</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B147">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C147">
-        <v>0.128</v>
+        <v>1.693</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B148">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C148">
-        <v>0.312</v>
+        <v>1.65</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B149">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C149">
-        <v>0.594</v>
+        <v>1.478</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B150">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C150">
-        <v>0.621</v>
+        <v>1.206</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B151">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C151">
-        <v>0.641</v>
+        <v>0.788</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B152">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C152">
-        <v>0.621</v>
+        <v>0.245</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B153">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C153">
-        <v>0.59</v>
+        <v>0.037</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B154">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C154">
-        <v>0.471</v>
+        <v>0.012</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B155">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C155">
-        <v>0.364</v>
+        <v>0.012</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B156">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C156">
-        <v>0.265</v>
+        <v>0.012</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B157">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C157">
-        <v>0.128</v>
+        <v>0.012</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B158">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C158">
-        <v>0.015</v>
+        <v>0.012</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B159">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C159">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B160">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C160">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B161">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C161">
         <v>0.013</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B162">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C162">
         <v>0.013</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B163">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C163">
         <v>0.013</v>
@@ -3184,10 +3184,10 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B164">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C164">
         <v>0.012</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B165">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C165">
-        <v>0.012</v>
+        <v>0.033</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B166">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C166">
-        <v>0.012</v>
+        <v>0.261</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B167">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C167">
-        <v>0.012</v>
+        <v>0.795</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B168">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C168">
-        <v>0.012</v>
+        <v>1.38</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B169">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C169">
-        <v>0.012</v>
+        <v>1.579</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B170">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C170">
-        <v>0.031</v>
+        <v>1.895</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Fixing the api_key_entsoe missing value
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,9 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>25.03.202512</t>
-  </si>
-  <si>
     <t>25.03.202513</t>
   </si>
   <si>
@@ -533,6 +530,9 @@
   </si>
   <si>
     <t>01.04.202512</t>
+  </si>
+  <si>
+    <t>01.04.202513</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
         <v>45741</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0.011</v>
@@ -933,10 +933,10 @@
         <v>45741</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>3.399</v>
+        <v>3.531</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -947,10 +947,10 @@
         <v>45741</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>2.446</v>
+        <v>2.134</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -961,10 +961,10 @@
         <v>45741</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>1.939</v>
+        <v>1.645</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -975,10 +975,10 @@
         <v>45741</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>1.924</v>
+        <v>1.251</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -989,10 +989,10 @@
         <v>45741</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>1.393</v>
+        <v>0.489</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45741</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>0.547</v>
+        <v>0.031</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
         <v>45741</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1031,10 +1031,10 @@
         <v>45741</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1045,10 +1045,10 @@
         <v>45741</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1059,10 +1059,10 @@
         <v>45741</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1073,10 +1073,10 @@
         <v>45741</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1101,10 +1101,10 @@
         <v>45742</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1115,10 +1115,10 @@
         <v>45742</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1129,10 +1129,10 @@
         <v>45742</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1143,10 +1143,10 @@
         <v>45742</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1157,10 +1157,10 @@
         <v>45742</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1171,7 +1171,7 @@
         <v>45742</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>0.012</v>
@@ -1185,10 +1185,10 @@
         <v>45742</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>0.022</v>
+        <v>0.246</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1199,10 +1199,10 @@
         <v>45742</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>0.301</v>
+        <v>0.795</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1213,10 +1213,10 @@
         <v>45742</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>0.793</v>
+        <v>1.252</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1227,10 +1227,10 @@
         <v>45742</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>1.249</v>
+        <v>1.388</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1241,10 +1241,10 @@
         <v>45742</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>1.381</v>
+        <v>1.447</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1255,10 +1255,10 @@
         <v>45742</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>1.408</v>
+        <v>1.552</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1269,10 +1269,10 @@
         <v>45742</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>1.427</v>
+        <v>1.38</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1283,10 +1283,10 @@
         <v>45742</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>1.388</v>
+        <v>1.071</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1297,10 +1297,10 @@
         <v>45742</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0.999</v>
+        <v>0.785</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1311,10 +1311,10 @@
         <v>45742</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0.76</v>
+        <v>0.369</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1325,10 +1325,10 @@
         <v>45742</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>0.346</v>
+        <v>0.125</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45742</v>
       </c>
       <c r="B32">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>0.128</v>
+        <v>0.012</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,10 +1353,10 @@
         <v>45742</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1367,10 +1367,10 @@
         <v>45742</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1381,10 +1381,10 @@
         <v>45742</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C35">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1395,10 +1395,10 @@
         <v>45742</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1409,10 +1409,10 @@
         <v>45742</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B38">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1437,10 +1437,10 @@
         <v>45743</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1451,10 +1451,10 @@
         <v>45743</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1465,10 +1465,10 @@
         <v>45743</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1479,10 +1479,10 @@
         <v>45743</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1493,10 +1493,10 @@
         <v>45743</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1507,10 +1507,10 @@
         <v>45743</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1521,10 +1521,10 @@
         <v>45743</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>0.013</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1535,10 +1535,10 @@
         <v>45743</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>0.061</v>
+        <v>0.212</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1549,10 +1549,10 @@
         <v>45743</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>0.204</v>
+        <v>0.381</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1563,10 +1563,10 @@
         <v>45743</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>0.334</v>
+        <v>0.68</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1577,10 +1577,10 @@
         <v>45743</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>0.621</v>
+        <v>0.838</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1591,10 +1591,10 @@
         <v>45743</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>0.798</v>
+        <v>0.888</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1605,10 +1605,10 @@
         <v>45743</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>0.805</v>
+        <v>0.8</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1619,10 +1619,10 @@
         <v>45743</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>0.801</v>
+        <v>0.67</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1633,10 +1633,10 @@
         <v>45743</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>0.737</v>
+        <v>0.616</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1647,10 +1647,10 @@
         <v>45743</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>0.637</v>
+        <v>0.358</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1661,10 +1661,10 @@
         <v>45743</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>0.368</v>
+        <v>0.123</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1675,10 +1675,10 @@
         <v>45743</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>0.128</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1689,10 +1689,10 @@
         <v>45743</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1703,10 +1703,10 @@
         <v>45743</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1717,10 +1717,10 @@
         <v>45743</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C59">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1731,10 +1731,10 @@
         <v>45743</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C60">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1745,10 +1745,10 @@
         <v>45743</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B62">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1773,10 +1773,10 @@
         <v>45744</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1787,10 +1787,10 @@
         <v>45744</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1801,10 +1801,10 @@
         <v>45744</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1815,10 +1815,10 @@
         <v>45744</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1829,10 +1829,10 @@
         <v>45744</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1843,10 +1843,10 @@
         <v>45744</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1857,10 +1857,10 @@
         <v>45744</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>0.015</v>
+        <v>0.061</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1871,10 +1871,10 @@
         <v>45744</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>0.091</v>
+        <v>0.203</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1885,10 +1885,10 @@
         <v>45744</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0.207</v>
+        <v>0.322</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1899,10 +1899,10 @@
         <v>45744</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>0.357</v>
+        <v>0.598</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1913,10 +1913,10 @@
         <v>45744</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>0.618</v>
+        <v>0.61</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1927,10 +1927,10 @@
         <v>45744</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C74">
-        <v>0.704</v>
+        <v>0.632</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1941,10 +1941,10 @@
         <v>45744</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>0.753</v>
+        <v>0.61</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1955,10 +1955,10 @@
         <v>45744</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>0.749</v>
+        <v>0.624</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1969,10 +1969,10 @@
         <v>45744</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>0.743</v>
+        <v>0.648</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1983,10 +1983,10 @@
         <v>45744</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>0.745</v>
+        <v>0.455</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1997,10 +1997,10 @@
         <v>45744</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>0.598</v>
+        <v>0.184</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45744</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C80">
-        <v>0.196</v>
+        <v>0.012</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,10 +2025,10 @@
         <v>45744</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>0.023</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2039,10 +2039,10 @@
         <v>45744</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2053,10 +2053,10 @@
         <v>45744</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C83">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2067,10 +2067,10 @@
         <v>45744</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C84">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2081,10 +2081,10 @@
         <v>45744</v>
       </c>
       <c r="B85">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C85">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45744</v>
+        <v>45745</v>
       </c>
       <c r="B86">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C86">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2109,10 +2109,10 @@
         <v>45745</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C87">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2123,10 +2123,10 @@
         <v>45745</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C88">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2137,10 +2137,10 @@
         <v>45745</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C89">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2151,10 +2151,10 @@
         <v>45745</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2165,10 +2165,10 @@
         <v>45745</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2179,10 +2179,10 @@
         <v>45745</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2193,10 +2193,10 @@
         <v>45745</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C93">
-        <v>0.015</v>
+        <v>0.096</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2207,10 +2207,10 @@
         <v>45745</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>0.12</v>
+        <v>0.274</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2221,10 +2221,10 @@
         <v>45745</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0.259</v>
+        <v>0.442</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2235,10 +2235,10 @@
         <v>45745</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C96">
-        <v>0.545</v>
+        <v>0.706</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2249,10 +2249,10 @@
         <v>45745</v>
       </c>
       <c r="B97">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>0.776</v>
+        <v>0.89</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2263,10 +2263,10 @@
         <v>45745</v>
       </c>
       <c r="B98">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>0.863</v>
+        <v>0.952</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2277,10 +2277,10 @@
         <v>45745</v>
       </c>
       <c r="B99">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>0.983</v>
+        <v>1.075</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2291,10 +2291,10 @@
         <v>45745</v>
       </c>
       <c r="B100">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C100">
-        <v>1.044</v>
+        <v>0.988</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2305,10 +2305,10 @@
         <v>45745</v>
       </c>
       <c r="B101">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>0.993</v>
+        <v>0.983</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2319,10 +2319,10 @@
         <v>45745</v>
       </c>
       <c r="B102">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C102">
-        <v>0.992</v>
+        <v>0.781</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2333,10 +2333,10 @@
         <v>45745</v>
       </c>
       <c r="B103">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>0.781</v>
+        <v>0.282</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45745</v>
       </c>
       <c r="B104">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C104">
-        <v>0.274</v>
+        <v>0.024</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,10 +2361,10 @@
         <v>45745</v>
       </c>
       <c r="B105">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>0.038</v>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2375,10 +2375,10 @@
         <v>45745</v>
       </c>
       <c r="B106">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2389,10 +2389,10 @@
         <v>45745</v>
       </c>
       <c r="B107">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2403,10 +2403,10 @@
         <v>45745</v>
       </c>
       <c r="B108">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2417,10 +2417,10 @@
         <v>45745</v>
       </c>
       <c r="B109">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C109">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45745</v>
+        <v>45746</v>
       </c>
       <c r="B110">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2445,10 +2445,10 @@
         <v>45746</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C111">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2459,10 +2459,10 @@
         <v>45746</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2473,10 +2473,10 @@
         <v>45746</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2487,10 +2487,10 @@
         <v>45746</v>
       </c>
       <c r="B114">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C114">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2501,10 +2501,10 @@
         <v>45746</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2515,10 +2515,10 @@
         <v>45746</v>
       </c>
       <c r="B116">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>0.012</v>
+        <v>0.022</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2529,10 +2529,10 @@
         <v>45746</v>
       </c>
       <c r="B117">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C117">
-        <v>0.031</v>
+        <v>0.286</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2543,10 +2543,10 @@
         <v>45746</v>
       </c>
       <c r="B118">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C118">
-        <v>0.305</v>
+        <v>1.039</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2557,10 +2557,10 @@
         <v>45746</v>
       </c>
       <c r="B119">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C119">
-        <v>0.9370000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2571,10 +2571,10 @@
         <v>45746</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C120">
-        <v>1.582</v>
+        <v>2.019</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2585,10 +2585,10 @@
         <v>45746</v>
       </c>
       <c r="B121">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C121">
-        <v>1.791</v>
+        <v>2.249</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2599,10 +2599,10 @@
         <v>45746</v>
       </c>
       <c r="B122">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>2.046</v>
+        <v>2.493</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2613,10 +2613,10 @@
         <v>45746</v>
       </c>
       <c r="B123">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>2.335</v>
+        <v>2.538</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2627,10 +2627,10 @@
         <v>45746</v>
       </c>
       <c r="B124">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C124">
-        <v>2.335</v>
+        <v>2.026</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2641,10 +2641,10 @@
         <v>45746</v>
       </c>
       <c r="B125">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C125">
-        <v>1.95</v>
+        <v>1.51</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2655,10 +2655,10 @@
         <v>45746</v>
       </c>
       <c r="B126">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C126">
-        <v>1.511</v>
+        <v>0.967</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2669,10 +2669,10 @@
         <v>45746</v>
       </c>
       <c r="B127">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C127">
-        <v>0.948</v>
+        <v>0.291</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2683,10 +2683,10 @@
         <v>45746</v>
       </c>
       <c r="B128">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C128">
-        <v>0.3</v>
+        <v>0.031</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,10 +2697,10 @@
         <v>45746</v>
       </c>
       <c r="B129">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>0.041</v>
+        <v>0</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2711,10 +2711,10 @@
         <v>45746</v>
       </c>
       <c r="B130">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2725,10 +2725,10 @@
         <v>45746</v>
       </c>
       <c r="B131">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C131">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2739,10 +2739,10 @@
         <v>45746</v>
       </c>
       <c r="B132">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C132">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2753,10 +2753,10 @@
         <v>45746</v>
       </c>
       <c r="B133">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C133">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45746</v>
+        <v>45747</v>
       </c>
       <c r="B134">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C134">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2781,10 +2781,10 @@
         <v>45747</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2795,10 +2795,10 @@
         <v>45747</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2809,10 +2809,10 @@
         <v>45747</v>
       </c>
       <c r="B137">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C137">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2823,10 +2823,10 @@
         <v>45747</v>
       </c>
       <c r="B138">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C138">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2837,10 +2837,10 @@
         <v>45747</v>
       </c>
       <c r="B139">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C139">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2851,10 +2851,10 @@
         <v>45747</v>
       </c>
       <c r="B140">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C140">
-        <v>0.012</v>
+        <v>0.016</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2865,10 +2865,10 @@
         <v>45747</v>
       </c>
       <c r="B141">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C141">
-        <v>0.022</v>
+        <v>0.18</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2879,10 +2879,10 @@
         <v>45747</v>
       </c>
       <c r="B142">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C142">
-        <v>0.202</v>
+        <v>0.602</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2893,10 +2893,10 @@
         <v>45747</v>
       </c>
       <c r="B143">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>0.625</v>
+        <v>1.153</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2907,10 +2907,10 @@
         <v>45747</v>
       </c>
       <c r="B144">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>0.996</v>
+        <v>1.538</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2921,10 +2921,10 @@
         <v>45747</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C145">
-        <v>1.452</v>
+        <v>1.67</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2935,10 +2935,10 @@
         <v>45747</v>
       </c>
       <c r="B146">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C146">
-        <v>1.605</v>
+        <v>1.841</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2949,10 +2949,10 @@
         <v>45747</v>
       </c>
       <c r="B147">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C147">
-        <v>1.693</v>
+        <v>1.71</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2963,10 +2963,10 @@
         <v>45747</v>
       </c>
       <c r="B148">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C148">
-        <v>1.65</v>
+        <v>1.536</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2977,10 +2977,10 @@
         <v>45747</v>
       </c>
       <c r="B149">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C149">
-        <v>1.478</v>
+        <v>1.297</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2991,10 +2991,10 @@
         <v>45747</v>
       </c>
       <c r="B150">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C150">
-        <v>1.206</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3005,10 +3005,10 @@
         <v>45747</v>
       </c>
       <c r="B151">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C151">
-        <v>0.788</v>
+        <v>0.243</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3019,10 +3019,10 @@
         <v>45747</v>
       </c>
       <c r="B152">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C152">
-        <v>0.245</v>
+        <v>0.025</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,10 +3033,10 @@
         <v>45747</v>
       </c>
       <c r="B153">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C153">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3047,10 +3047,10 @@
         <v>45747</v>
       </c>
       <c r="B154">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3061,10 +3061,10 @@
         <v>45747</v>
       </c>
       <c r="B155">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C155">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3075,10 +3075,10 @@
         <v>45747</v>
       </c>
       <c r="B156">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C156">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3089,10 +3089,10 @@
         <v>45747</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C157">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45747</v>
+        <v>45748</v>
       </c>
       <c r="B158">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3117,10 +3117,10 @@
         <v>45748</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C159">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3131,10 +3131,10 @@
         <v>45748</v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C160">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3145,10 +3145,10 @@
         <v>45748</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C161">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3159,10 +3159,10 @@
         <v>45748</v>
       </c>
       <c r="B162">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C162">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3173,10 +3173,10 @@
         <v>45748</v>
       </c>
       <c r="B163">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3187,10 +3187,10 @@
         <v>45748</v>
       </c>
       <c r="B164">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C164">
-        <v>0.012</v>
+        <v>0.024</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3201,10 +3201,10 @@
         <v>45748</v>
       </c>
       <c r="B165">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C165">
-        <v>0.033</v>
+        <v>0.258</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3215,10 +3215,10 @@
         <v>45748</v>
       </c>
       <c r="B166">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C166">
-        <v>0.261</v>
+        <v>0.841</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3229,10 +3229,10 @@
         <v>45748</v>
       </c>
       <c r="B167">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C167">
-        <v>0.795</v>
+        <v>1.547</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3243,10 +3243,10 @@
         <v>45748</v>
       </c>
       <c r="B168">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C168">
-        <v>1.38</v>
+        <v>1.78</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3257,10 +3257,10 @@
         <v>45748</v>
       </c>
       <c r="B169">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C169">
-        <v>1.579</v>
+        <v>2.102</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3271,10 +3271,10 @@
         <v>45748</v>
       </c>
       <c r="B170">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C170">
-        <v>1.895</v>
+        <v>2.178</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Improving the Kahraman forecast results by applying an April correctioin for month March
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,9 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>25.03.202513</t>
-  </si>
-  <si>
     <t>25.03.202514</t>
   </si>
   <si>
@@ -533,6 +530,9 @@
   </si>
   <si>
     <t>01.04.202513</t>
+  </si>
+  <si>
+    <t>01.04.202514</t>
   </si>
 </sst>
 </file>
@@ -919,10 +919,10 @@
         <v>45741</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -933,10 +933,10 @@
         <v>45741</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>3.531</v>
+        <v>1.805</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -947,10 +947,10 @@
         <v>45741</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>2.134</v>
+        <v>0.914</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -961,10 +961,10 @@
         <v>45741</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>1.645</v>
+        <v>1.009</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -975,10 +975,10 @@
         <v>45741</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>1.251</v>
+        <v>0.393</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -989,10 +989,10 @@
         <v>45741</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>0.489</v>
+        <v>0.034</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45741</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>0.031</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,7 +1017,7 @@
         <v>45741</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>45741</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1045,7 +1045,7 @@
         <v>45741</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1059,7 +1059,7 @@
         <v>45741</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1087,7 +1087,7 @@
         <v>45742</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1101,7 +1101,7 @@
         <v>45742</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1115,7 +1115,7 @@
         <v>45742</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>45742</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>45742</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1157,10 +1157,10 @@
         <v>45742</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1171,10 +1171,10 @@
         <v>45742</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>0.012</v>
+        <v>0.27</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1185,10 +1185,10 @@
         <v>45742</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0.246</v>
+        <v>0.876</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1199,10 +1199,10 @@
         <v>45742</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>0.795</v>
+        <v>1.303</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1213,10 +1213,10 @@
         <v>45742</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>1.252</v>
+        <v>1.328</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1227,10 +1227,10 @@
         <v>45742</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>1.388</v>
+        <v>1.408</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1241,10 +1241,10 @@
         <v>45742</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <v>1.447</v>
+        <v>1.307</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1255,10 +1255,10 @@
         <v>45742</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>1.552</v>
+        <v>1.01</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1269,10 +1269,10 @@
         <v>45742</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>1.38</v>
+        <v>0.805</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1283,10 +1283,10 @@
         <v>45742</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>1.071</v>
+        <v>0.656</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1297,10 +1297,10 @@
         <v>45742</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>0.785</v>
+        <v>0.344</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1311,10 +1311,10 @@
         <v>45742</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30">
-        <v>0.369</v>
+        <v>0.127</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1325,10 +1325,10 @@
         <v>45742</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>0.125</v>
+        <v>0.01</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45742</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,7 +1353,7 @@
         <v>45742</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1367,7 +1367,7 @@
         <v>45742</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1381,7 +1381,7 @@
         <v>45742</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1395,7 +1395,7 @@
         <v>45742</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="B37">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1423,7 +1423,7 @@
         <v>45743</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>45743</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>45743</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1465,7 +1465,7 @@
         <v>45743</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>45743</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>45743</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1507,10 +1507,10 @@
         <v>45743</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1521,10 +1521,10 @@
         <v>45743</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0.08599999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1535,10 +1535,10 @@
         <v>45743</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>0.212</v>
+        <v>0.669</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1549,10 +1549,10 @@
         <v>45743</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C47">
-        <v>0.381</v>
+        <v>0.872</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1563,10 +1563,10 @@
         <v>45743</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>0.68</v>
+        <v>1.003</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1577,10 +1577,10 @@
         <v>45743</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>0.838</v>
+        <v>1.042</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1591,10 +1591,10 @@
         <v>45743</v>
       </c>
       <c r="B50">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C50">
-        <v>0.888</v>
+        <v>0.993</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1605,10 +1605,10 @@
         <v>45743</v>
       </c>
       <c r="B51">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51">
-        <v>0.8</v>
+        <v>0.773</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1619,10 +1619,10 @@
         <v>45743</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>0.67</v>
+        <v>0.708</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1633,10 +1633,10 @@
         <v>45743</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>0.616</v>
+        <v>0.394</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1647,10 +1647,10 @@
         <v>45743</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C54">
-        <v>0.358</v>
+        <v>0.135</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1661,10 +1661,10 @@
         <v>45743</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C55">
-        <v>0.123</v>
+        <v>0.01</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1675,7 +1675,7 @@
         <v>45743</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1689,7 +1689,7 @@
         <v>45743</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>45743</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>45743</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>45743</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="B61">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1759,7 +1759,7 @@
         <v>45744</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1773,7 +1773,7 @@
         <v>45744</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>45744</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1801,7 +1801,7 @@
         <v>45744</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>45744</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1829,7 +1829,7 @@
         <v>45744</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1843,10 +1843,10 @@
         <v>45744</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1857,10 +1857,10 @@
         <v>45744</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>0.061</v>
+        <v>0.223</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1871,10 +1871,10 @@
         <v>45744</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C70">
-        <v>0.203</v>
+        <v>0.407</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1885,10 +1885,10 @@
         <v>45744</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>0.322</v>
+        <v>0.672</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1899,10 +1899,10 @@
         <v>45744</v>
       </c>
       <c r="B72">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>0.598</v>
+        <v>0.727</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1913,10 +1913,10 @@
         <v>45744</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C73">
-        <v>0.61</v>
+        <v>0.697</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1927,10 +1927,10 @@
         <v>45744</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>0.632</v>
+        <v>0.651</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1941,10 +1941,10 @@
         <v>45744</v>
       </c>
       <c r="B75">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>0.61</v>
+        <v>0.643</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1955,10 +1955,10 @@
         <v>45744</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C76">
-        <v>0.624</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1969,10 +1969,10 @@
         <v>45744</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>0.648</v>
+        <v>0.605</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1983,10 +1983,10 @@
         <v>45744</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>0.455</v>
+        <v>0.203</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1997,10 +1997,10 @@
         <v>45744</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C79">
-        <v>0.184</v>
+        <v>0.013</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45744</v>
       </c>
       <c r="B80">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>0.012</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,7 +2025,7 @@
         <v>45744</v>
       </c>
       <c r="B81">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>45744</v>
       </c>
       <c r="B82">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2053,7 +2053,7 @@
         <v>45744</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>45744</v>
       </c>
       <c r="B84">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45744</v>
+        <v>45745</v>
       </c>
       <c r="B85">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>45745</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2109,7 +2109,7 @@
         <v>45745</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>45745</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>45745</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>45745</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2165,7 +2165,7 @@
         <v>45745</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2179,10 +2179,10 @@
         <v>45745</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.105</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2193,10 +2193,10 @@
         <v>45745</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C93">
-        <v>0.096</v>
+        <v>0.291</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2207,10 +2207,10 @@
         <v>45745</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C94">
-        <v>0.274</v>
+        <v>0.661</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2221,10 +2221,10 @@
         <v>45745</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C95">
-        <v>0.442</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2235,10 +2235,10 @@
         <v>45745</v>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C96">
-        <v>0.706</v>
+        <v>0.958</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2249,10 +2249,10 @@
         <v>45745</v>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C97">
-        <v>0.89</v>
+        <v>1.01</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2263,10 +2263,10 @@
         <v>45745</v>
       </c>
       <c r="B98">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C98">
-        <v>0.952</v>
+        <v>0.954</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2277,10 +2277,10 @@
         <v>45745</v>
       </c>
       <c r="B99">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C99">
-        <v>1.075</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2291,10 +2291,10 @@
         <v>45745</v>
       </c>
       <c r="B100">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C100">
-        <v>0.988</v>
+        <v>1.034</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2305,10 +2305,10 @@
         <v>45745</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C101">
-        <v>0.983</v>
+        <v>0.864</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2319,10 +2319,10 @@
         <v>45745</v>
       </c>
       <c r="B102">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>0.781</v>
+        <v>0.309</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2333,10 +2333,10 @@
         <v>45745</v>
       </c>
       <c r="B103">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C103">
-        <v>0.282</v>
+        <v>0.027</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45745</v>
       </c>
       <c r="B104">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C104">
-        <v>0.024</v>
+        <v>0</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,7 +2361,7 @@
         <v>45745</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2375,7 +2375,7 @@
         <v>45745</v>
       </c>
       <c r="B106">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2389,7 +2389,7 @@
         <v>45745</v>
       </c>
       <c r="B107">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2403,7 +2403,7 @@
         <v>45745</v>
       </c>
       <c r="B108">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45745</v>
+        <v>45746</v>
       </c>
       <c r="B109">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2431,7 +2431,7 @@
         <v>45746</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         <v>45746</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2459,7 +2459,7 @@
         <v>45746</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>45746</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2487,7 +2487,7 @@
         <v>45746</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2501,10 +2501,10 @@
         <v>45746</v>
       </c>
       <c r="B115">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.017</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2515,10 +2515,10 @@
         <v>45746</v>
       </c>
       <c r="B116">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C116">
-        <v>0.022</v>
+        <v>0.27</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2529,10 +2529,10 @@
         <v>45746</v>
       </c>
       <c r="B117">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C117">
-        <v>0.286</v>
+        <v>0.998</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2543,10 +2543,10 @@
         <v>45746</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C118">
-        <v>1.039</v>
+        <v>1.707</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2557,10 +2557,10 @@
         <v>45746</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C119">
-        <v>1.55</v>
+        <v>2.121</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2571,10 +2571,10 @@
         <v>45746</v>
       </c>
       <c r="B120">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C120">
-        <v>2.019</v>
+        <v>2.588</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2585,10 +2585,10 @@
         <v>45746</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C121">
-        <v>2.249</v>
+        <v>2.736</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2599,10 +2599,10 @@
         <v>45746</v>
       </c>
       <c r="B122">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C122">
-        <v>2.493</v>
+        <v>2.802</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2613,10 +2613,10 @@
         <v>45746</v>
       </c>
       <c r="B123">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C123">
-        <v>2.538</v>
+        <v>2.732</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2627,10 +2627,10 @@
         <v>45746</v>
       </c>
       <c r="B124">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C124">
-        <v>2.026</v>
+        <v>1.886</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2641,10 +2641,10 @@
         <v>45746</v>
       </c>
       <c r="B125">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C125">
-        <v>1.51</v>
+        <v>1.192</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2655,10 +2655,10 @@
         <v>45746</v>
       </c>
       <c r="B126">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C126">
-        <v>0.967</v>
+        <v>0.32</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2669,10 +2669,10 @@
         <v>45746</v>
       </c>
       <c r="B127">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C127">
-        <v>0.291</v>
+        <v>0.034</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2683,10 +2683,10 @@
         <v>45746</v>
       </c>
       <c r="B128">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C128">
-        <v>0.031</v>
+        <v>0</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,7 +2697,7 @@
         <v>45746</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2711,7 +2711,7 @@
         <v>45746</v>
       </c>
       <c r="B130">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2725,7 +2725,7 @@
         <v>45746</v>
       </c>
       <c r="B131">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2739,7 +2739,7 @@
         <v>45746</v>
       </c>
       <c r="B132">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45746</v>
+        <v>45747</v>
       </c>
       <c r="B133">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2767,7 +2767,7 @@
         <v>45747</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2781,7 +2781,7 @@
         <v>45747</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2795,7 +2795,7 @@
         <v>45747</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2809,7 +2809,7 @@
         <v>45747</v>
       </c>
       <c r="B137">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>45747</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2837,10 +2837,10 @@
         <v>45747</v>
       </c>
       <c r="B139">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2851,10 +2851,10 @@
         <v>45747</v>
       </c>
       <c r="B140">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C140">
-        <v>0.016</v>
+        <v>0.161</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2865,10 +2865,10 @@
         <v>45747</v>
       </c>
       <c r="B141">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C141">
-        <v>0.18</v>
+        <v>0.397</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2879,10 +2879,10 @@
         <v>45747</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C142">
-        <v>0.602</v>
+        <v>0.909</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2893,10 +2893,10 @@
         <v>45747</v>
       </c>
       <c r="B143">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C143">
-        <v>1.153</v>
+        <v>1.353</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2907,10 +2907,10 @@
         <v>45747</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C144">
-        <v>1.538</v>
+        <v>1.757</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2921,10 +2921,10 @@
         <v>45747</v>
       </c>
       <c r="B145">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C145">
-        <v>1.67</v>
+        <v>1.73</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2935,10 +2935,10 @@
         <v>45747</v>
       </c>
       <c r="B146">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C146">
-        <v>1.841</v>
+        <v>1.697</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2949,10 +2949,10 @@
         <v>45747</v>
       </c>
       <c r="B147">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C147">
-        <v>1.71</v>
+        <v>1.63</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2963,10 +2963,10 @@
         <v>45747</v>
       </c>
       <c r="B148">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C148">
-        <v>1.536</v>
+        <v>1.293</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2977,10 +2977,10 @@
         <v>45747</v>
       </c>
       <c r="B149">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C149">
-        <v>1.297</v>
+        <v>0.741</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2991,10 +2991,10 @@
         <v>45747</v>
       </c>
       <c r="B150">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C150">
-        <v>0.8149999999999999</v>
+        <v>0.208</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3005,10 +3005,10 @@
         <v>45747</v>
       </c>
       <c r="B151">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C151">
-        <v>0.243</v>
+        <v>0.027</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3019,10 +3019,10 @@
         <v>45747</v>
       </c>
       <c r="B152">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C152">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,7 +3033,7 @@
         <v>45747</v>
       </c>
       <c r="B153">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -3047,7 +3047,7 @@
         <v>45747</v>
       </c>
       <c r="B154">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -3061,7 +3061,7 @@
         <v>45747</v>
       </c>
       <c r="B155">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3075,7 +3075,7 @@
         <v>45747</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45747</v>
+        <v>45748</v>
       </c>
       <c r="B157">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3103,7 +3103,7 @@
         <v>45748</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3117,7 +3117,7 @@
         <v>45748</v>
       </c>
       <c r="B159">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3131,7 +3131,7 @@
         <v>45748</v>
       </c>
       <c r="B160">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3145,7 +3145,7 @@
         <v>45748</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3159,7 +3159,7 @@
         <v>45748</v>
       </c>
       <c r="B162">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -3173,10 +3173,10 @@
         <v>45748</v>
       </c>
       <c r="B163">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3187,10 +3187,10 @@
         <v>45748</v>
       </c>
       <c r="B164">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C164">
-        <v>0.024</v>
+        <v>0.208</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3201,10 +3201,10 @@
         <v>45748</v>
       </c>
       <c r="B165">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C165">
-        <v>0.258</v>
+        <v>0.727</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3215,10 +3215,10 @@
         <v>45748</v>
       </c>
       <c r="B166">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C166">
-        <v>0.841</v>
+        <v>1.301</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3229,10 +3229,10 @@
         <v>45748</v>
       </c>
       <c r="B167">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C167">
-        <v>1.547</v>
+        <v>1.528</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3243,10 +3243,10 @@
         <v>45748</v>
       </c>
       <c r="B168">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C168">
-        <v>1.78</v>
+        <v>1.584</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3257,10 +3257,10 @@
         <v>45748</v>
       </c>
       <c r="B169">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C169">
-        <v>2.102</v>
+        <v>1.699</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3271,10 +3271,10 @@
         <v>45748</v>
       </c>
       <c r="B170">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C170">
-        <v>2.178</v>
+        <v>1.686</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Switching to Summer time
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,228 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>25.03.202514</t>
-  </si>
-  <si>
-    <t>25.03.202515</t>
-  </si>
-  <si>
-    <t>25.03.202516</t>
-  </si>
-  <si>
-    <t>25.03.202517</t>
-  </si>
-  <si>
-    <t>25.03.202518</t>
-  </si>
-  <si>
-    <t>25.03.202519</t>
-  </si>
-  <si>
-    <t>25.03.202520</t>
-  </si>
-  <si>
-    <t>25.03.202521</t>
-  </si>
-  <si>
-    <t>25.03.202522</t>
-  </si>
-  <si>
-    <t>25.03.202523</t>
-  </si>
-  <si>
-    <t>25.03.202524</t>
-  </si>
-  <si>
-    <t>26.03.20251</t>
-  </si>
-  <si>
-    <t>26.03.20252</t>
-  </si>
-  <si>
-    <t>26.03.20253</t>
-  </si>
-  <si>
-    <t>26.03.20254</t>
-  </si>
-  <si>
-    <t>26.03.20255</t>
-  </si>
-  <si>
-    <t>26.03.20256</t>
-  </si>
-  <si>
-    <t>26.03.20257</t>
-  </si>
-  <si>
-    <t>26.03.20258</t>
-  </si>
-  <si>
-    <t>26.03.20259</t>
-  </si>
-  <si>
-    <t>26.03.202510</t>
-  </si>
-  <si>
-    <t>26.03.202511</t>
-  </si>
-  <si>
-    <t>26.03.202512</t>
-  </si>
-  <si>
-    <t>26.03.202513</t>
-  </si>
-  <si>
-    <t>26.03.202514</t>
-  </si>
-  <si>
-    <t>26.03.202515</t>
-  </si>
-  <si>
-    <t>26.03.202516</t>
-  </si>
-  <si>
-    <t>26.03.202517</t>
-  </si>
-  <si>
-    <t>26.03.202518</t>
-  </si>
-  <si>
-    <t>26.03.202519</t>
-  </si>
-  <si>
-    <t>26.03.202520</t>
-  </si>
-  <si>
-    <t>26.03.202521</t>
-  </si>
-  <si>
-    <t>26.03.202522</t>
-  </si>
-  <si>
-    <t>26.03.202523</t>
-  </si>
-  <si>
-    <t>26.03.202524</t>
-  </si>
-  <si>
-    <t>27.03.20251</t>
-  </si>
-  <si>
-    <t>27.03.20252</t>
-  </si>
-  <si>
-    <t>27.03.20253</t>
-  </si>
-  <si>
-    <t>27.03.20254</t>
-  </si>
-  <si>
-    <t>27.03.20255</t>
-  </si>
-  <si>
-    <t>27.03.20256</t>
-  </si>
-  <si>
-    <t>27.03.20257</t>
-  </si>
-  <si>
-    <t>27.03.20258</t>
-  </si>
-  <si>
-    <t>27.03.20259</t>
-  </si>
-  <si>
-    <t>27.03.202510</t>
-  </si>
-  <si>
-    <t>27.03.202511</t>
-  </si>
-  <si>
-    <t>27.03.202512</t>
-  </si>
-  <si>
-    <t>27.03.202513</t>
-  </si>
-  <si>
-    <t>27.03.202514</t>
-  </si>
-  <si>
-    <t>27.03.202515</t>
-  </si>
-  <si>
-    <t>27.03.202516</t>
-  </si>
-  <si>
-    <t>27.03.202517</t>
-  </si>
-  <si>
-    <t>27.03.202518</t>
-  </si>
-  <si>
-    <t>27.03.202519</t>
-  </si>
-  <si>
-    <t>27.03.202520</t>
-  </si>
-  <si>
-    <t>27.03.202521</t>
-  </si>
-  <si>
-    <t>27.03.202522</t>
-  </si>
-  <si>
-    <t>27.03.202523</t>
-  </si>
-  <si>
-    <t>27.03.202524</t>
-  </si>
-  <si>
-    <t>28.03.20251</t>
-  </si>
-  <si>
-    <t>28.03.20252</t>
-  </si>
-  <si>
-    <t>28.03.20253</t>
-  </si>
-  <si>
-    <t>28.03.20254</t>
-  </si>
-  <si>
-    <t>28.03.20255</t>
-  </si>
-  <si>
-    <t>28.03.20256</t>
-  </si>
-  <si>
-    <t>28.03.20257</t>
-  </si>
-  <si>
-    <t>28.03.20258</t>
-  </si>
-  <si>
-    <t>28.03.20259</t>
-  </si>
-  <si>
-    <t>28.03.202510</t>
-  </si>
-  <si>
-    <t>28.03.202511</t>
-  </si>
-  <si>
-    <t>28.03.202512</t>
-  </si>
-  <si>
-    <t>28.03.202513</t>
-  </si>
-  <si>
-    <t>28.03.202514</t>
-  </si>
-  <si>
-    <t>28.03.202515</t>
-  </si>
-  <si>
     <t>28.03.202516</t>
   </si>
   <si>
@@ -533,6 +311,228 @@
   </si>
   <si>
     <t>01.04.202514</t>
+  </si>
+  <si>
+    <t>01.04.202515</t>
+  </si>
+  <si>
+    <t>01.04.202516</t>
+  </si>
+  <si>
+    <t>01.04.202517</t>
+  </si>
+  <si>
+    <t>01.04.202518</t>
+  </si>
+  <si>
+    <t>01.04.202519</t>
+  </si>
+  <si>
+    <t>01.04.202520</t>
+  </si>
+  <si>
+    <t>01.04.202521</t>
+  </si>
+  <si>
+    <t>01.04.202522</t>
+  </si>
+  <si>
+    <t>01.04.202523</t>
+  </si>
+  <si>
+    <t>01.04.202524</t>
+  </si>
+  <si>
+    <t>02.04.20251</t>
+  </si>
+  <si>
+    <t>02.04.20252</t>
+  </si>
+  <si>
+    <t>02.04.20253</t>
+  </si>
+  <si>
+    <t>02.04.20254</t>
+  </si>
+  <si>
+    <t>02.04.20255</t>
+  </si>
+  <si>
+    <t>02.04.20256</t>
+  </si>
+  <si>
+    <t>02.04.20257</t>
+  </si>
+  <si>
+    <t>02.04.20258</t>
+  </si>
+  <si>
+    <t>02.04.20259</t>
+  </si>
+  <si>
+    <t>02.04.202510</t>
+  </si>
+  <si>
+    <t>02.04.202511</t>
+  </si>
+  <si>
+    <t>02.04.202512</t>
+  </si>
+  <si>
+    <t>02.04.202513</t>
+  </si>
+  <si>
+    <t>02.04.202514</t>
+  </si>
+  <si>
+    <t>02.04.202515</t>
+  </si>
+  <si>
+    <t>02.04.202516</t>
+  </si>
+  <si>
+    <t>02.04.202517</t>
+  </si>
+  <si>
+    <t>02.04.202518</t>
+  </si>
+  <si>
+    <t>02.04.202519</t>
+  </si>
+  <si>
+    <t>02.04.202520</t>
+  </si>
+  <si>
+    <t>02.04.202521</t>
+  </si>
+  <si>
+    <t>02.04.202522</t>
+  </si>
+  <si>
+    <t>02.04.202523</t>
+  </si>
+  <si>
+    <t>02.04.202524</t>
+  </si>
+  <si>
+    <t>03.04.20251</t>
+  </si>
+  <si>
+    <t>03.04.20252</t>
+  </si>
+  <si>
+    <t>03.04.20253</t>
+  </si>
+  <si>
+    <t>03.04.20254</t>
+  </si>
+  <si>
+    <t>03.04.20255</t>
+  </si>
+  <si>
+    <t>03.04.20256</t>
+  </si>
+  <si>
+    <t>03.04.20257</t>
+  </si>
+  <si>
+    <t>03.04.20258</t>
+  </si>
+  <si>
+    <t>03.04.20259</t>
+  </si>
+  <si>
+    <t>03.04.202510</t>
+  </si>
+  <si>
+    <t>03.04.202511</t>
+  </si>
+  <si>
+    <t>03.04.202512</t>
+  </si>
+  <si>
+    <t>03.04.202513</t>
+  </si>
+  <si>
+    <t>03.04.202514</t>
+  </si>
+  <si>
+    <t>03.04.202515</t>
+  </si>
+  <si>
+    <t>03.04.202516</t>
+  </si>
+  <si>
+    <t>03.04.202517</t>
+  </si>
+  <si>
+    <t>03.04.202518</t>
+  </si>
+  <si>
+    <t>03.04.202519</t>
+  </si>
+  <si>
+    <t>03.04.202520</t>
+  </si>
+  <si>
+    <t>03.04.202521</t>
+  </si>
+  <si>
+    <t>03.04.202522</t>
+  </si>
+  <si>
+    <t>03.04.202523</t>
+  </si>
+  <si>
+    <t>03.04.202524</t>
+  </si>
+  <si>
+    <t>04.04.20251</t>
+  </si>
+  <si>
+    <t>04.04.20252</t>
+  </si>
+  <si>
+    <t>04.04.20253</t>
+  </si>
+  <si>
+    <t>04.04.20254</t>
+  </si>
+  <si>
+    <t>04.04.20255</t>
+  </si>
+  <si>
+    <t>04.04.20256</t>
+  </si>
+  <si>
+    <t>04.04.20257</t>
+  </si>
+  <si>
+    <t>04.04.20258</t>
+  </si>
+  <si>
+    <t>04.04.20259</t>
+  </si>
+  <si>
+    <t>04.04.202510</t>
+  </si>
+  <si>
+    <t>04.04.202511</t>
+  </si>
+  <si>
+    <t>04.04.202512</t>
+  </si>
+  <si>
+    <t>04.04.202513</t>
+  </si>
+  <si>
+    <t>04.04.202514</t>
+  </si>
+  <si>
+    <t>04.04.202515</t>
+  </si>
+  <si>
+    <t>04.04.202516</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0.012</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>1.805</v>
+        <v>0.012</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>0.914</v>
+        <v>0.221</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>1.009</v>
+        <v>0.095</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>0.393</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45741</v>
+        <v>45745</v>
       </c>
       <c r="B12">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>0.013</v>
+        <v>0.068</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>0.27</v>
+        <v>0.223</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>0.876</v>
+        <v>0.306</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>1.303</v>
+        <v>0.415</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C23">
-        <v>1.328</v>
+        <v>0.651</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C24">
-        <v>1.408</v>
+        <v>0.671</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>1.307</v>
+        <v>0.663</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>1.01</v>
+        <v>0.639</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C27">
-        <v>0.805</v>
+        <v>0.643</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>0.656</v>
+        <v>0.467</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C29">
-        <v>0.344</v>
+        <v>0.205</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C30">
-        <v>0.127</v>
+        <v>0.024</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C31">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45742</v>
+        <v>45746</v>
       </c>
       <c r="B36">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>0.065</v>
+        <v>1.298</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>0.22</v>
+        <v>2.127</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>0.669</v>
+        <v>2.696</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C47">
-        <v>0.872</v>
+        <v>3.548</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C48">
-        <v>1.003</v>
+        <v>3.69</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C49">
-        <v>1.042</v>
+        <v>3.564</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C50">
-        <v>0.993</v>
+        <v>2.426</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>0.773</v>
+        <v>2.148</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C52">
-        <v>0.708</v>
+        <v>1.566</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C53">
-        <v>0.394</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>0.135</v>
+        <v>0.061</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C55">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1700,10 +1700,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="B60">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.024</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.273</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>0.068</v>
+        <v>0.718</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C69">
-        <v>0.223</v>
+        <v>1.196</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C70">
-        <v>0.407</v>
+        <v>1.419</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C71">
-        <v>0.672</v>
+        <v>1.695</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C72">
-        <v>0.727</v>
+        <v>1.735</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C73">
-        <v>0.697</v>
+        <v>1.728</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C74">
-        <v>0.651</v>
+        <v>1.679</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C75">
-        <v>0.643</v>
+        <v>1.519</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C76">
-        <v>0.6820000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C77">
-        <v>0.605</v>
+        <v>0.316</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C78">
-        <v>0.203</v>
+        <v>0.034</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C79">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,10 +2008,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2022,10 +2022,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2036,10 +2036,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2064,10 +2064,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B88">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.213</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C92">
-        <v>0.105</v>
+        <v>0.412</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C93">
-        <v>0.291</v>
+        <v>0.771</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C94">
-        <v>0.661</v>
+        <v>1.042</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B95">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C95">
-        <v>0.8129999999999999</v>
+        <v>1.412</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C96">
-        <v>0.958</v>
+        <v>1.627</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C97">
-        <v>1.01</v>
+        <v>1.715</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B98">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C98">
-        <v>0.954</v>
+        <v>1.501</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B99">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C99">
-        <v>0.9350000000000001</v>
+        <v>1.601</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C100">
-        <v>1.034</v>
+        <v>1.17</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B101">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C101">
-        <v>0.864</v>
+        <v>0.478</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B102">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C102">
-        <v>0.309</v>
+        <v>0.061</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B103">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C103">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,10 +2344,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B105">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B106">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45745</v>
+        <v>45749</v>
       </c>
       <c r="B107">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45745</v>
+        <v>45749</v>
       </c>
       <c r="B108">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B112">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B115">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C115">
-        <v>0.017</v>
+        <v>0.703</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B116">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C116">
-        <v>0.27</v>
+        <v>1.594</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B117">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C117">
-        <v>0.998</v>
+        <v>2.671</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B118">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C118">
-        <v>1.707</v>
+        <v>3.625</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B119">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C119">
-        <v>2.121</v>
+        <v>3.833</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B120">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C120">
-        <v>2.588</v>
+        <v>3.644</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B121">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C121">
-        <v>2.736</v>
+        <v>3.462</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B122">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C122">
-        <v>2.802</v>
+        <v>3.419</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B123">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C123">
-        <v>2.732</v>
+        <v>2.344</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B124">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C124">
-        <v>1.886</v>
+        <v>1.673</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B125">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C125">
-        <v>1.192</v>
+        <v>0.744</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B126">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C126">
-        <v>0.32</v>
+        <v>0.099</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B127">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C127">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,10 +2680,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -2694,10 +2694,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B129">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B130">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45746</v>
+        <v>45750</v>
       </c>
       <c r="B131">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45746</v>
+        <v>45750</v>
       </c>
       <c r="B132">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B135">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B136">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B138">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>0.062</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B139">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C139">
-        <v>0.013</v>
+        <v>0.781</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B140">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C140">
-        <v>0.161</v>
+        <v>1.928</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B141">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C141">
-        <v>0.397</v>
+        <v>2.78</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B142">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C142">
-        <v>0.909</v>
+        <v>3.801</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C143">
-        <v>1.353</v>
+        <v>4.272</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B144">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C144">
-        <v>1.757</v>
+        <v>4.307</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B145">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C145">
-        <v>1.73</v>
+        <v>4.031</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B146">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C146">
-        <v>1.697</v>
+        <v>3.45</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B147">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C147">
-        <v>1.63</v>
+        <v>2.535</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B148">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C148">
-        <v>1.293</v>
+        <v>1.596</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B149">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C149">
-        <v>0.741</v>
+        <v>0.705</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B150">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C150">
-        <v>0.208</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B151">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C151">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,10 +3016,10 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B152">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -3030,10 +3030,10 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B153">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B154">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45747</v>
+        <v>45751</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45747</v>
+        <v>45751</v>
       </c>
       <c r="B156">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B158">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B159">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B160">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B161">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B162">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B163">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C163">
-        <v>0.023</v>
+        <v>0.656</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B164">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C164">
-        <v>0.208</v>
+        <v>1.714</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B165">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C165">
-        <v>0.727</v>
+        <v>2.696</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B166">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C166">
-        <v>1.301</v>
+        <v>3.444</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B167">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C167">
-        <v>1.528</v>
+        <v>3.624</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B168">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C168">
-        <v>1.584</v>
+        <v>3.811</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B169">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C169">
-        <v>1.699</v>
+        <v>3.779</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B170">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C170">
-        <v>1.686</v>
+        <v>3.243</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Fixing the huge difference between the hourly and quarterly forecasted values
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,201 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>28.03.202516</t>
-  </si>
-  <si>
-    <t>28.03.202517</t>
-  </si>
-  <si>
-    <t>28.03.202518</t>
-  </si>
-  <si>
-    <t>28.03.202519</t>
-  </si>
-  <si>
-    <t>28.03.202520</t>
-  </si>
-  <si>
-    <t>28.03.202521</t>
-  </si>
-  <si>
-    <t>28.03.202522</t>
-  </si>
-  <si>
-    <t>28.03.202523</t>
-  </si>
-  <si>
-    <t>28.03.202524</t>
-  </si>
-  <si>
-    <t>29.03.20251</t>
-  </si>
-  <si>
-    <t>29.03.20252</t>
-  </si>
-  <si>
-    <t>29.03.20253</t>
-  </si>
-  <si>
-    <t>29.03.20254</t>
-  </si>
-  <si>
-    <t>29.03.20255</t>
-  </si>
-  <si>
-    <t>29.03.20256</t>
-  </si>
-  <si>
-    <t>29.03.20257</t>
-  </si>
-  <si>
-    <t>29.03.20258</t>
-  </si>
-  <si>
-    <t>29.03.20259</t>
-  </si>
-  <si>
-    <t>29.03.202510</t>
-  </si>
-  <si>
-    <t>29.03.202511</t>
-  </si>
-  <si>
-    <t>29.03.202512</t>
-  </si>
-  <si>
-    <t>29.03.202513</t>
-  </si>
-  <si>
-    <t>29.03.202514</t>
-  </si>
-  <si>
-    <t>29.03.202515</t>
-  </si>
-  <si>
-    <t>29.03.202516</t>
-  </si>
-  <si>
-    <t>29.03.202517</t>
-  </si>
-  <si>
-    <t>29.03.202518</t>
-  </si>
-  <si>
-    <t>29.03.202519</t>
-  </si>
-  <si>
-    <t>29.03.202520</t>
-  </si>
-  <si>
-    <t>29.03.202521</t>
-  </si>
-  <si>
-    <t>29.03.202522</t>
-  </si>
-  <si>
-    <t>29.03.202523</t>
-  </si>
-  <si>
-    <t>29.03.202524</t>
-  </si>
-  <si>
-    <t>30.03.20251</t>
-  </si>
-  <si>
-    <t>30.03.20252</t>
-  </si>
-  <si>
-    <t>30.03.20253</t>
-  </si>
-  <si>
-    <t>30.03.20254</t>
-  </si>
-  <si>
-    <t>30.03.20255</t>
-  </si>
-  <si>
-    <t>30.03.20256</t>
-  </si>
-  <si>
-    <t>30.03.20257</t>
-  </si>
-  <si>
-    <t>30.03.20258</t>
-  </si>
-  <si>
-    <t>30.03.20259</t>
-  </si>
-  <si>
-    <t>30.03.202510</t>
-  </si>
-  <si>
-    <t>30.03.202511</t>
-  </si>
-  <si>
-    <t>30.03.202512</t>
-  </si>
-  <si>
-    <t>30.03.202513</t>
-  </si>
-  <si>
-    <t>30.03.202514</t>
-  </si>
-  <si>
-    <t>30.03.202515</t>
-  </si>
-  <si>
-    <t>30.03.202516</t>
-  </si>
-  <si>
-    <t>30.03.202517</t>
-  </si>
-  <si>
-    <t>30.03.202518</t>
-  </si>
-  <si>
-    <t>30.03.202519</t>
-  </si>
-  <si>
-    <t>30.03.202520</t>
-  </si>
-  <si>
-    <t>30.03.202521</t>
-  </si>
-  <si>
-    <t>30.03.202522</t>
-  </si>
-  <si>
-    <t>30.03.202523</t>
-  </si>
-  <si>
-    <t>30.03.202524</t>
-  </si>
-  <si>
-    <t>31.03.20251</t>
-  </si>
-  <si>
-    <t>31.03.20252</t>
-  </si>
-  <si>
-    <t>31.03.20253</t>
-  </si>
-  <si>
-    <t>31.03.20254</t>
-  </si>
-  <si>
-    <t>31.03.20255</t>
-  </si>
-  <si>
-    <t>31.03.20256</t>
-  </si>
-  <si>
-    <t>31.03.20257</t>
-  </si>
-  <si>
-    <t>31.03.20258</t>
-  </si>
-  <si>
     <t>31.03.20259</t>
   </si>
   <si>
@@ -533,6 +338,201 @@
   </si>
   <si>
     <t>04.04.202516</t>
+  </si>
+  <si>
+    <t>04.04.202517</t>
+  </si>
+  <si>
+    <t>04.04.202518</t>
+  </si>
+  <si>
+    <t>04.04.202519</t>
+  </si>
+  <si>
+    <t>04.04.202520</t>
+  </si>
+  <si>
+    <t>04.04.202521</t>
+  </si>
+  <si>
+    <t>04.04.202522</t>
+  </si>
+  <si>
+    <t>04.04.202523</t>
+  </si>
+  <si>
+    <t>04.04.202524</t>
+  </si>
+  <si>
+    <t>05.04.20251</t>
+  </si>
+  <si>
+    <t>05.04.20252</t>
+  </si>
+  <si>
+    <t>05.04.20253</t>
+  </si>
+  <si>
+    <t>05.04.20254</t>
+  </si>
+  <si>
+    <t>05.04.20255</t>
+  </si>
+  <si>
+    <t>05.04.20256</t>
+  </si>
+  <si>
+    <t>05.04.20257</t>
+  </si>
+  <si>
+    <t>05.04.20258</t>
+  </si>
+  <si>
+    <t>05.04.20259</t>
+  </si>
+  <si>
+    <t>05.04.202510</t>
+  </si>
+  <si>
+    <t>05.04.202511</t>
+  </si>
+  <si>
+    <t>05.04.202512</t>
+  </si>
+  <si>
+    <t>05.04.202513</t>
+  </si>
+  <si>
+    <t>05.04.202514</t>
+  </si>
+  <si>
+    <t>05.04.202515</t>
+  </si>
+  <si>
+    <t>05.04.202516</t>
+  </si>
+  <si>
+    <t>05.04.202517</t>
+  </si>
+  <si>
+    <t>05.04.202518</t>
+  </si>
+  <si>
+    <t>05.04.202519</t>
+  </si>
+  <si>
+    <t>05.04.202520</t>
+  </si>
+  <si>
+    <t>05.04.202521</t>
+  </si>
+  <si>
+    <t>05.04.202522</t>
+  </si>
+  <si>
+    <t>05.04.202523</t>
+  </si>
+  <si>
+    <t>05.04.202524</t>
+  </si>
+  <si>
+    <t>06.04.20251</t>
+  </si>
+  <si>
+    <t>06.04.20252</t>
+  </si>
+  <si>
+    <t>06.04.20253</t>
+  </si>
+  <si>
+    <t>06.04.20254</t>
+  </si>
+  <si>
+    <t>06.04.20255</t>
+  </si>
+  <si>
+    <t>06.04.20256</t>
+  </si>
+  <si>
+    <t>06.04.20257</t>
+  </si>
+  <si>
+    <t>06.04.20258</t>
+  </si>
+  <si>
+    <t>06.04.20259</t>
+  </si>
+  <si>
+    <t>06.04.202510</t>
+  </si>
+  <si>
+    <t>06.04.202511</t>
+  </si>
+  <si>
+    <t>06.04.202512</t>
+  </si>
+  <si>
+    <t>06.04.202513</t>
+  </si>
+  <si>
+    <t>06.04.202514</t>
+  </si>
+  <si>
+    <t>06.04.202515</t>
+  </si>
+  <si>
+    <t>06.04.202516</t>
+  </si>
+  <si>
+    <t>06.04.202517</t>
+  </si>
+  <si>
+    <t>06.04.202518</t>
+  </si>
+  <si>
+    <t>06.04.202519</t>
+  </si>
+  <si>
+    <t>06.04.202520</t>
+  </si>
+  <si>
+    <t>06.04.202521</t>
+  </si>
+  <si>
+    <t>06.04.202522</t>
+  </si>
+  <si>
+    <t>06.04.202523</t>
+  </si>
+  <si>
+    <t>06.04.202524</t>
+  </si>
+  <si>
+    <t>07.04.20251</t>
+  </si>
+  <si>
+    <t>07.04.20252</t>
+  </si>
+  <si>
+    <t>07.04.20253</t>
+  </si>
+  <si>
+    <t>07.04.20254</t>
+  </si>
+  <si>
+    <t>07.04.20255</t>
+  </si>
+  <si>
+    <t>07.04.20256</t>
+  </si>
+  <si>
+    <t>07.04.20257</t>
+  </si>
+  <si>
+    <t>07.04.20258</t>
+  </si>
+  <si>
+    <t>07.04.20259</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>0.221</v>
+        <v>1.336</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>0.095</v>
+        <v>1.802</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2.433</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2.598</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2.703</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2.267</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1.679</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.351</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.031</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45745</v>
+        <v>45747</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>0.068</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>0.223</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B21">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>0.306</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>0.415</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>0.651</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B24">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>0.671</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>0.663</v>
+        <v>0.016</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B26">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>0.639</v>
+        <v>0.187</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B27">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>0.643</v>
+        <v>0.592</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B28">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C28">
-        <v>0.467</v>
+        <v>0.989</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B29">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C29">
-        <v>0.205</v>
+        <v>1.276</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B30">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>0.024</v>
+        <v>1.518</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B31">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1.699</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1.449</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B33">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1.312</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="B34">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1.287</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.906</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.343</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45746</v>
+        <v>45748</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>0.5669999999999999</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>1.298</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C45">
-        <v>2.127</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B46">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C46">
-        <v>2.696</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B47">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>3.548</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>3.69</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B49">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>3.564</v>
+        <v>0.033</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B50">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C50">
-        <v>2.426</v>
+        <v>0.524</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B51">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C51">
-        <v>2.148</v>
+        <v>1.479</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C52">
-        <v>1.566</v>
+        <v>2.417</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C53">
-        <v>0.5570000000000001</v>
+        <v>3.2</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B54">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C54">
-        <v>0.061</v>
+        <v>3.303</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B55">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>3.336</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B56">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3.186</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B57">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>2.731</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45746</v>
+        <v>45749</v>
       </c>
       <c r="B58">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2.207</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1.442</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.508</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45747</v>
+        <v>45749</v>
       </c>
       <c r="B65">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B66">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>0.024</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B67">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C67">
-        <v>0.273</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B68">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>0.718</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B69">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>1.196</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C70">
-        <v>1.419</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B71">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>1.695</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B72">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C72">
-        <v>1.735</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B73">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C73">
-        <v>1.728</v>
+        <v>0.021</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B74">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C74">
-        <v>1.679</v>
+        <v>0.164</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B75">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C75">
-        <v>1.519</v>
+        <v>0.322</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B76">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C76">
-        <v>1.01</v>
+        <v>0.652</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B77">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C77">
-        <v>0.316</v>
+        <v>0.863</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B78">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C78">
-        <v>0.034</v>
+        <v>0.92</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B79">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>0.909</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B80">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.726</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B81">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45747</v>
+        <v>45750</v>
       </c>
       <c r="B82">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.707</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.577</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B85">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.031</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B88">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45748</v>
+        <v>45750</v>
       </c>
       <c r="B89">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C90">
-        <v>0.023</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B91">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C91">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B92">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C92">
-        <v>0.412</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B93">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C93">
-        <v>0.771</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B94">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>1.042</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B95">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>1.412</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B96">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>1.627</v>
+        <v>0</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B97">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C97">
-        <v>1.715</v>
+        <v>0.055</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B98">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C98">
-        <v>1.501</v>
+        <v>0.554</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B99">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>1.601</v>
+        <v>1.389</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B100">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C100">
-        <v>1.17</v>
+        <v>2.188</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B101">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C101">
-        <v>0.478</v>
+        <v>2.521</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B102">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C102">
-        <v>0.061</v>
+        <v>2.988</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B103">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>2.955</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B104">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>2.756</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B105">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>2.547</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45748</v>
+        <v>45751</v>
       </c>
       <c r="B106">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>2.088</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1.46</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.533</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B110">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B111">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B112">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45749</v>
+        <v>45751</v>
       </c>
       <c r="B113">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B114">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C114">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B115">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C115">
-        <v>0.703</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B116">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>1.594</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B117">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>2.671</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B118">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C118">
-        <v>3.625</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B119">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>3.833</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B120">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C120">
-        <v>3.644</v>
+        <v>0</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B121">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C121">
-        <v>3.462</v>
+        <v>0.058</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B122">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C122">
-        <v>3.419</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B123">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C123">
-        <v>2.344</v>
+        <v>1.237</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B124">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C124">
-        <v>1.673</v>
+        <v>1.83</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B125">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C125">
-        <v>0.744</v>
+        <v>2.192</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B126">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C126">
-        <v>0.099</v>
+        <v>2.519</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B127">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>2.557</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B128">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B129">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>2.017</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45749</v>
+        <v>45752</v>
       </c>
       <c r="B130">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>1.51</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.963</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B132">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.347</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.058</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B134">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B135">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B136">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45750</v>
+        <v>45752</v>
       </c>
       <c r="B137">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B138">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C138">
-        <v>0.062</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B139">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C139">
-        <v>0.781</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B140">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C140">
-        <v>1.928</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B141">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C141">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B142">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C142">
-        <v>3.801</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B143">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C143">
-        <v>4.272</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B144">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C144">
-        <v>4.307</v>
+        <v>0</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B145">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C145">
-        <v>4.031</v>
+        <v>0.058</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B146">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C146">
-        <v>3.45</v>
+        <v>0.596</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B147">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C147">
-        <v>2.535</v>
+        <v>1.277</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B148">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C148">
-        <v>1.596</v>
+        <v>2.04</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B149">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C149">
-        <v>0.705</v>
+        <v>2.659</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B150">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C150">
-        <v>0.08799999999999999</v>
+        <v>2.602</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B151">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>2.623</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B152">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>2.683</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B153">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>2.466</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45750</v>
+        <v>45753</v>
       </c>
       <c r="B154">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>1.241</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B156">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.603</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B157">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.098</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B158">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B159">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B160">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45751</v>
+        <v>45753</v>
       </c>
       <c r="B161">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B162">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C162">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B163">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C163">
-        <v>0.656</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B164">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C164">
-        <v>1.714</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B165">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>2.696</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B166">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C166">
-        <v>3.444</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B167">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C167">
-        <v>3.624</v>
+        <v>0</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B168">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C168">
-        <v>3.811</v>
+        <v>0</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B169">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C169">
-        <v>3.779</v>
+        <v>0.058</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45751</v>
+        <v>45754</v>
       </c>
       <c r="B170">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C170">
-        <v>3.243</v>
+        <v>0.463</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Replacing the Kahraman model with a new one
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,390 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>31.03.202513</t>
-  </si>
-  <si>
-    <t>31.03.202514</t>
-  </si>
-  <si>
-    <t>31.03.202515</t>
-  </si>
-  <si>
-    <t>31.03.202516</t>
-  </si>
-  <si>
-    <t>31.03.202517</t>
-  </si>
-  <si>
-    <t>31.03.202518</t>
-  </si>
-  <si>
-    <t>31.03.202519</t>
-  </si>
-  <si>
-    <t>31.03.202520</t>
-  </si>
-  <si>
-    <t>31.03.202521</t>
-  </si>
-  <si>
-    <t>31.03.202522</t>
-  </si>
-  <si>
-    <t>31.03.202523</t>
-  </si>
-  <si>
-    <t>31.03.202524</t>
-  </si>
-  <si>
-    <t>01.04.20251</t>
-  </si>
-  <si>
-    <t>01.04.20252</t>
-  </si>
-  <si>
-    <t>01.04.20253</t>
-  </si>
-  <si>
-    <t>01.04.20254</t>
-  </si>
-  <si>
-    <t>01.04.20255</t>
-  </si>
-  <si>
-    <t>01.04.20256</t>
-  </si>
-  <si>
-    <t>01.04.20257</t>
-  </si>
-  <si>
-    <t>01.04.20258</t>
-  </si>
-  <si>
-    <t>01.04.20259</t>
-  </si>
-  <si>
-    <t>01.04.202510</t>
-  </si>
-  <si>
-    <t>01.04.202511</t>
-  </si>
-  <si>
-    <t>01.04.202512</t>
-  </si>
-  <si>
-    <t>01.04.202513</t>
-  </si>
-  <si>
-    <t>01.04.202514</t>
-  </si>
-  <si>
-    <t>01.04.202515</t>
-  </si>
-  <si>
-    <t>01.04.202516</t>
-  </si>
-  <si>
-    <t>01.04.202517</t>
-  </si>
-  <si>
-    <t>01.04.202518</t>
-  </si>
-  <si>
-    <t>01.04.202519</t>
-  </si>
-  <si>
-    <t>01.04.202520</t>
-  </si>
-  <si>
-    <t>01.04.202521</t>
-  </si>
-  <si>
-    <t>01.04.202522</t>
-  </si>
-  <si>
-    <t>01.04.202523</t>
-  </si>
-  <si>
-    <t>01.04.202524</t>
-  </si>
-  <si>
-    <t>02.04.20251</t>
-  </si>
-  <si>
-    <t>02.04.20252</t>
-  </si>
-  <si>
-    <t>02.04.20253</t>
-  </si>
-  <si>
-    <t>02.04.20254</t>
-  </si>
-  <si>
-    <t>02.04.20255</t>
-  </si>
-  <si>
-    <t>02.04.20256</t>
-  </si>
-  <si>
-    <t>02.04.20257</t>
-  </si>
-  <si>
-    <t>02.04.20258</t>
-  </si>
-  <si>
-    <t>02.04.20259</t>
-  </si>
-  <si>
-    <t>02.04.202510</t>
-  </si>
-  <si>
-    <t>02.04.202511</t>
-  </si>
-  <si>
-    <t>02.04.202512</t>
-  </si>
-  <si>
-    <t>02.04.202513</t>
-  </si>
-  <si>
-    <t>02.04.202514</t>
-  </si>
-  <si>
-    <t>02.04.202515</t>
-  </si>
-  <si>
-    <t>02.04.202516</t>
-  </si>
-  <si>
-    <t>02.04.202517</t>
-  </si>
-  <si>
-    <t>02.04.202518</t>
-  </si>
-  <si>
-    <t>02.04.202519</t>
-  </si>
-  <si>
-    <t>02.04.202520</t>
-  </si>
-  <si>
-    <t>02.04.202521</t>
-  </si>
-  <si>
-    <t>02.04.202522</t>
-  </si>
-  <si>
-    <t>02.04.202523</t>
-  </si>
-  <si>
-    <t>02.04.202524</t>
-  </si>
-  <si>
-    <t>03.04.20251</t>
-  </si>
-  <si>
-    <t>03.04.20252</t>
-  </si>
-  <si>
-    <t>03.04.20253</t>
-  </si>
-  <si>
-    <t>03.04.20254</t>
-  </si>
-  <si>
-    <t>03.04.20255</t>
-  </si>
-  <si>
-    <t>03.04.20256</t>
-  </si>
-  <si>
-    <t>03.04.20257</t>
-  </si>
-  <si>
-    <t>03.04.20258</t>
-  </si>
-  <si>
-    <t>03.04.20259</t>
-  </si>
-  <si>
-    <t>03.04.202510</t>
-  </si>
-  <si>
-    <t>03.04.202511</t>
-  </si>
-  <si>
-    <t>03.04.202512</t>
-  </si>
-  <si>
-    <t>03.04.202513</t>
-  </si>
-  <si>
-    <t>03.04.202514</t>
-  </si>
-  <si>
-    <t>03.04.202515</t>
-  </si>
-  <si>
-    <t>03.04.202516</t>
-  </si>
-  <si>
-    <t>03.04.202517</t>
-  </si>
-  <si>
-    <t>03.04.202518</t>
-  </si>
-  <si>
-    <t>03.04.202519</t>
-  </si>
-  <si>
-    <t>03.04.202520</t>
-  </si>
-  <si>
-    <t>03.04.202521</t>
-  </si>
-  <si>
-    <t>03.04.202522</t>
-  </si>
-  <si>
-    <t>03.04.202523</t>
-  </si>
-  <si>
-    <t>03.04.202524</t>
-  </si>
-  <si>
-    <t>04.04.20251</t>
-  </si>
-  <si>
-    <t>04.04.20252</t>
-  </si>
-  <si>
-    <t>04.04.20253</t>
-  </si>
-  <si>
-    <t>04.04.20254</t>
-  </si>
-  <si>
-    <t>04.04.20255</t>
-  </si>
-  <si>
-    <t>04.04.20256</t>
-  </si>
-  <si>
-    <t>04.04.20257</t>
-  </si>
-  <si>
-    <t>04.04.20258</t>
-  </si>
-  <si>
-    <t>04.04.20259</t>
-  </si>
-  <si>
-    <t>04.04.202510</t>
-  </si>
-  <si>
-    <t>04.04.202511</t>
-  </si>
-  <si>
-    <t>04.04.202512</t>
-  </si>
-  <si>
-    <t>04.04.202513</t>
-  </si>
-  <si>
-    <t>04.04.202514</t>
-  </si>
-  <si>
-    <t>04.04.202515</t>
-  </si>
-  <si>
-    <t>04.04.202516</t>
-  </si>
-  <si>
-    <t>04.04.202517</t>
-  </si>
-  <si>
-    <t>04.04.202518</t>
-  </si>
-  <si>
-    <t>04.04.202519</t>
-  </si>
-  <si>
-    <t>04.04.202520</t>
-  </si>
-  <si>
-    <t>04.04.202521</t>
-  </si>
-  <si>
-    <t>04.04.202522</t>
-  </si>
-  <si>
-    <t>04.04.202523</t>
-  </si>
-  <si>
-    <t>04.04.202524</t>
-  </si>
-  <si>
-    <t>05.04.20251</t>
-  </si>
-  <si>
-    <t>05.04.20252</t>
-  </si>
-  <si>
-    <t>05.04.20253</t>
-  </si>
-  <si>
-    <t>05.04.20254</t>
-  </si>
-  <si>
-    <t>05.04.20255</t>
-  </si>
-  <si>
-    <t>05.04.20256</t>
-  </si>
-  <si>
-    <t>05.04.20257</t>
-  </si>
-  <si>
-    <t>05.04.20258</t>
-  </si>
-  <si>
-    <t>05.04.20259</t>
-  </si>
-  <si>
-    <t>05.04.202510</t>
-  </si>
-  <si>
-    <t>05.04.202511</t>
-  </si>
-  <si>
-    <t>05.04.202512</t>
-  </si>
-  <si>
-    <t>05.04.202513</t>
-  </si>
-  <si>
-    <t>05.04.202514</t>
-  </si>
-  <si>
-    <t>05.04.202515</t>
-  </si>
-  <si>
-    <t>05.04.202516</t>
-  </si>
-  <si>
-    <t>05.04.202517</t>
-  </si>
-  <si>
-    <t>05.04.202518</t>
-  </si>
-  <si>
-    <t>05.04.202519</t>
-  </si>
-  <si>
-    <t>05.04.202520</t>
-  </si>
-  <si>
     <t>05.04.202521</t>
   </si>
   <si>
@@ -533,6 +149,390 @@
   </si>
   <si>
     <t>07.04.202513</t>
+  </si>
+  <si>
+    <t>07.04.202514</t>
+  </si>
+  <si>
+    <t>07.04.202515</t>
+  </si>
+  <si>
+    <t>07.04.202516</t>
+  </si>
+  <si>
+    <t>07.04.202517</t>
+  </si>
+  <si>
+    <t>07.04.202518</t>
+  </si>
+  <si>
+    <t>07.04.202519</t>
+  </si>
+  <si>
+    <t>07.04.202520</t>
+  </si>
+  <si>
+    <t>07.04.202521</t>
+  </si>
+  <si>
+    <t>07.04.202522</t>
+  </si>
+  <si>
+    <t>07.04.202523</t>
+  </si>
+  <si>
+    <t>07.04.202524</t>
+  </si>
+  <si>
+    <t>08.04.20251</t>
+  </si>
+  <si>
+    <t>08.04.20252</t>
+  </si>
+  <si>
+    <t>08.04.20253</t>
+  </si>
+  <si>
+    <t>08.04.20254</t>
+  </si>
+  <si>
+    <t>08.04.20255</t>
+  </si>
+  <si>
+    <t>08.04.20256</t>
+  </si>
+  <si>
+    <t>08.04.20257</t>
+  </si>
+  <si>
+    <t>08.04.20258</t>
+  </si>
+  <si>
+    <t>08.04.20259</t>
+  </si>
+  <si>
+    <t>08.04.202510</t>
+  </si>
+  <si>
+    <t>08.04.202511</t>
+  </si>
+  <si>
+    <t>08.04.202512</t>
+  </si>
+  <si>
+    <t>08.04.202513</t>
+  </si>
+  <si>
+    <t>08.04.202514</t>
+  </si>
+  <si>
+    <t>08.04.202515</t>
+  </si>
+  <si>
+    <t>08.04.202516</t>
+  </si>
+  <si>
+    <t>08.04.202517</t>
+  </si>
+  <si>
+    <t>08.04.202518</t>
+  </si>
+  <si>
+    <t>08.04.202519</t>
+  </si>
+  <si>
+    <t>08.04.202520</t>
+  </si>
+  <si>
+    <t>08.04.202521</t>
+  </si>
+  <si>
+    <t>08.04.202522</t>
+  </si>
+  <si>
+    <t>08.04.202523</t>
+  </si>
+  <si>
+    <t>08.04.202524</t>
+  </si>
+  <si>
+    <t>09.04.20251</t>
+  </si>
+  <si>
+    <t>09.04.20252</t>
+  </si>
+  <si>
+    <t>09.04.20253</t>
+  </si>
+  <si>
+    <t>09.04.20254</t>
+  </si>
+  <si>
+    <t>09.04.20255</t>
+  </si>
+  <si>
+    <t>09.04.20256</t>
+  </si>
+  <si>
+    <t>09.04.20257</t>
+  </si>
+  <si>
+    <t>09.04.20258</t>
+  </si>
+  <si>
+    <t>09.04.20259</t>
+  </si>
+  <si>
+    <t>09.04.202510</t>
+  </si>
+  <si>
+    <t>09.04.202511</t>
+  </si>
+  <si>
+    <t>09.04.202512</t>
+  </si>
+  <si>
+    <t>09.04.202513</t>
+  </si>
+  <si>
+    <t>09.04.202514</t>
+  </si>
+  <si>
+    <t>09.04.202515</t>
+  </si>
+  <si>
+    <t>09.04.202516</t>
+  </si>
+  <si>
+    <t>09.04.202517</t>
+  </si>
+  <si>
+    <t>09.04.202518</t>
+  </si>
+  <si>
+    <t>09.04.202519</t>
+  </si>
+  <si>
+    <t>09.04.202520</t>
+  </si>
+  <si>
+    <t>09.04.202521</t>
+  </si>
+  <si>
+    <t>09.04.202522</t>
+  </si>
+  <si>
+    <t>09.04.202523</t>
+  </si>
+  <si>
+    <t>09.04.202524</t>
+  </si>
+  <si>
+    <t>10.04.20251</t>
+  </si>
+  <si>
+    <t>10.04.20252</t>
+  </si>
+  <si>
+    <t>10.04.20253</t>
+  </si>
+  <si>
+    <t>10.04.20254</t>
+  </si>
+  <si>
+    <t>10.04.20255</t>
+  </si>
+  <si>
+    <t>10.04.20256</t>
+  </si>
+  <si>
+    <t>10.04.20257</t>
+  </si>
+  <si>
+    <t>10.04.20258</t>
+  </si>
+  <si>
+    <t>10.04.20259</t>
+  </si>
+  <si>
+    <t>10.04.202510</t>
+  </si>
+  <si>
+    <t>10.04.202511</t>
+  </si>
+  <si>
+    <t>10.04.202512</t>
+  </si>
+  <si>
+    <t>10.04.202513</t>
+  </si>
+  <si>
+    <t>10.04.202514</t>
+  </si>
+  <si>
+    <t>10.04.202515</t>
+  </si>
+  <si>
+    <t>10.04.202516</t>
+  </si>
+  <si>
+    <t>10.04.202517</t>
+  </si>
+  <si>
+    <t>10.04.202518</t>
+  </si>
+  <si>
+    <t>10.04.202519</t>
+  </si>
+  <si>
+    <t>10.04.202520</t>
+  </si>
+  <si>
+    <t>10.04.202521</t>
+  </si>
+  <si>
+    <t>10.04.202522</t>
+  </si>
+  <si>
+    <t>10.04.202523</t>
+  </si>
+  <si>
+    <t>10.04.202524</t>
+  </si>
+  <si>
+    <t>11.04.20251</t>
+  </si>
+  <si>
+    <t>11.04.20252</t>
+  </si>
+  <si>
+    <t>11.04.20253</t>
+  </si>
+  <si>
+    <t>11.04.20254</t>
+  </si>
+  <si>
+    <t>11.04.20255</t>
+  </si>
+  <si>
+    <t>11.04.20256</t>
+  </si>
+  <si>
+    <t>11.04.20257</t>
+  </si>
+  <si>
+    <t>11.04.20258</t>
+  </si>
+  <si>
+    <t>11.04.20259</t>
+  </si>
+  <si>
+    <t>11.04.202510</t>
+  </si>
+  <si>
+    <t>11.04.202511</t>
+  </si>
+  <si>
+    <t>11.04.202512</t>
+  </si>
+  <si>
+    <t>11.04.202513</t>
+  </si>
+  <si>
+    <t>11.04.202514</t>
+  </si>
+  <si>
+    <t>11.04.202515</t>
+  </si>
+  <si>
+    <t>11.04.202516</t>
+  </si>
+  <si>
+    <t>11.04.202517</t>
+  </si>
+  <si>
+    <t>11.04.202518</t>
+  </si>
+  <si>
+    <t>11.04.202519</t>
+  </si>
+  <si>
+    <t>11.04.202520</t>
+  </si>
+  <si>
+    <t>11.04.202521</t>
+  </si>
+  <si>
+    <t>11.04.202522</t>
+  </si>
+  <si>
+    <t>11.04.202523</t>
+  </si>
+  <si>
+    <t>11.04.202524</t>
+  </si>
+  <si>
+    <t>12.04.20251</t>
+  </si>
+  <si>
+    <t>12.04.20252</t>
+  </si>
+  <si>
+    <t>12.04.20253</t>
+  </si>
+  <si>
+    <t>12.04.20254</t>
+  </si>
+  <si>
+    <t>12.04.20255</t>
+  </si>
+  <si>
+    <t>12.04.20256</t>
+  </si>
+  <si>
+    <t>12.04.20257</t>
+  </si>
+  <si>
+    <t>12.04.20258</t>
+  </si>
+  <si>
+    <t>12.04.20259</t>
+  </si>
+  <si>
+    <t>12.04.202510</t>
+  </si>
+  <si>
+    <t>12.04.202511</t>
+  </si>
+  <si>
+    <t>12.04.202512</t>
+  </si>
+  <si>
+    <t>12.04.202513</t>
+  </si>
+  <si>
+    <t>12.04.202514</t>
+  </si>
+  <si>
+    <t>12.04.202515</t>
+  </si>
+  <si>
+    <t>12.04.202516</t>
+  </si>
+  <si>
+    <t>12.04.202517</t>
+  </si>
+  <si>
+    <t>12.04.202518</t>
+  </si>
+  <si>
+    <t>12.04.202519</t>
+  </si>
+  <si>
+    <t>12.04.202520</t>
+  </si>
+  <si>
+    <t>12.04.202521</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45747</v>
+        <v>45752</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>0.066</v>
+        <v>0.045</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45747</v>
+        <v>45752</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>0.066</v>
+        <v>0.045</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45747</v>
+        <v>45752</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>3.56</v>
+        <v>0.033</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45747</v>
+        <v>45752</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>2.917</v>
+        <v>0.033</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1.813</v>
+        <v>0.033</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1.011</v>
+        <v>0.033</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>0.442</v>
+        <v>0.033</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>0.055</v>
+        <v>0.033</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45747</v>
+        <v>45753</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>0.033</v>
+        <v>0.217</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>0.033</v>
+        <v>1.113</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>0.033</v>
+        <v>2.72</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>0.033</v>
+        <v>4.04</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>0.033</v>
+        <v>4.288</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>0.033</v>
+        <v>4.284</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>0.033</v>
+        <v>4.087</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>0.033</v>
+        <v>3.574</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <v>0.036</v>
+        <v>3.329</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <v>0.239</v>
+        <v>2.895</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>0.6919999999999999</v>
+        <v>2.044</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C24">
-        <v>1.069</v>
+        <v>0.894</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C25">
-        <v>1.52</v>
+        <v>0.223</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C26">
-        <v>1.505</v>
+        <v>0.039</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>1.524</v>
+        <v>0.033</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C28">
-        <v>1.523</v>
+        <v>0.033</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C29">
-        <v>1.278</v>
+        <v>0.033</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1.001</v>
+        <v>0.034</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>0.837</v>
+        <v>0.034</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>0.326</v>
+        <v>0.035</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C33">
-        <v>0.055</v>
+        <v>0.036</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C34">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45748</v>
+        <v>45754</v>
       </c>
       <c r="B37">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>0.033</v>
+        <v>0.218</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C38">
-        <v>0.033</v>
+        <v>1.014</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C39">
-        <v>0.033</v>
+        <v>2.114</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>0.033</v>
+        <v>3.116</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>0.033</v>
+        <v>3.625</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>0.033</v>
+        <v>3.841</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>0.033</v>
+        <v>3.838</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C44">
-        <v>0.033</v>
+        <v>3.474</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C45">
-        <v>0.056</v>
+        <v>2.964</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C46">
-        <v>0.602</v>
+        <v>2.189</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C47">
-        <v>1.625</v>
+        <v>1.512</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C48">
-        <v>2.525</v>
+        <v>0.636</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C49">
-        <v>3.394</v>
+        <v>0.099</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B50">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C50">
-        <v>3.669</v>
+        <v>0.042</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B51">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C51">
-        <v>3.726</v>
+        <v>0.041</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C52">
-        <v>3.584</v>
+        <v>0.039</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45749</v>
+        <v>45754</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C53">
-        <v>3.057</v>
+        <v>0.039</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>2.391</v>
+        <v>0.036</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1.631</v>
+        <v>0.036</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>0.737</v>
+        <v>0.036</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C57">
-        <v>0.096</v>
+        <v>0.036</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C58">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C59">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C60">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45749</v>
+        <v>45755</v>
       </c>
       <c r="B61">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C61">
-        <v>0.033</v>
+        <v>0.158</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>0.033</v>
+        <v>0.915</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C63">
-        <v>0.033</v>
+        <v>1.862</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>0.033</v>
+        <v>3.022</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C65">
-        <v>0.033</v>
+        <v>3.824</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C66">
-        <v>0.033</v>
+        <v>4.016</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C67">
-        <v>0.033</v>
+        <v>4.067</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C68">
-        <v>0.033</v>
+        <v>3.937</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C69">
-        <v>0.033</v>
+        <v>3.655</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C70">
-        <v>0.163</v>
+        <v>2.892</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C71">
-        <v>0.372</v>
+        <v>1.73</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B72">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C72">
-        <v>0.6929999999999999</v>
+        <v>0.786</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C73">
-        <v>0.966</v>
+        <v>0.152</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C74">
-        <v>1.308</v>
+        <v>0.039</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B75">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C75">
-        <v>1.548</v>
+        <v>0.039</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C76">
-        <v>1.439</v>
+        <v>0.034</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45750</v>
+        <v>45755</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C77">
-        <v>1.428</v>
+        <v>0.033</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C78">
-        <v>1.286</v>
+        <v>0.033</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C79">
-        <v>0.928</v>
+        <v>0.034</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B80">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C80">
-        <v>0.394</v>
+        <v>0.034</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B81">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C81">
-        <v>0.065</v>
+        <v>0.034</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B82">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C82">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C83">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B84">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C84">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45750</v>
+        <v>45756</v>
       </c>
       <c r="B85">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C85">
-        <v>0.033</v>
+        <v>0.222</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C86">
-        <v>0.033</v>
+        <v>1.014</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C87">
-        <v>0.033</v>
+        <v>2.31</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C88">
-        <v>0.033</v>
+        <v>3.496</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C89">
-        <v>0.033</v>
+        <v>4.57</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C90">
-        <v>0.033</v>
+        <v>4.437</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C91">
-        <v>0.033</v>
+        <v>4.306</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C92">
-        <v>0.033</v>
+        <v>3.731</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C93">
-        <v>0.083</v>
+        <v>3.074</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C94">
-        <v>0.733</v>
+        <v>2.393</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C95">
-        <v>1.699</v>
+        <v>1.675</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C96">
-        <v>2.748</v>
+        <v>0.764</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C97">
-        <v>3.194</v>
+        <v>0.152</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B98">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C98">
-        <v>3.704</v>
+        <v>0.039</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B99">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C99">
-        <v>3.803</v>
+        <v>0.033</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B100">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C100">
-        <v>3.559</v>
+        <v>0.033</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45751</v>
+        <v>45756</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C101">
-        <v>3.07</v>
+        <v>0.033</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B102">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>2.449</v>
+        <v>0.033</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B103">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C103">
-        <v>1.667</v>
+        <v>0.033</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B104">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C104">
-        <v>0.724</v>
+        <v>0.033</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C105">
-        <v>0.096</v>
+        <v>0.033</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B106">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C106">
         <v>0.033</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B107">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C107">
         <v>0.033</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B108">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C108">
         <v>0.033</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45751</v>
+        <v>45757</v>
       </c>
       <c r="B109">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C109">
-        <v>0.033</v>
+        <v>0.154</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C110">
-        <v>0.033</v>
+        <v>0.75</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C111">
-        <v>0.033</v>
+        <v>1.657</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C112">
-        <v>0.033</v>
+        <v>2.19</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C113">
-        <v>0.033</v>
+        <v>2.877</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C114">
-        <v>0.033</v>
+        <v>3.006</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B115">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C115">
-        <v>0.033</v>
+        <v>3.127</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B116">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C116">
-        <v>0.033</v>
+        <v>3.006</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B117">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C117">
-        <v>0.097</v>
+        <v>2.863</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C118">
-        <v>0.757</v>
+        <v>2.356</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C119">
-        <v>1.687</v>
+        <v>1.726</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B120">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C120">
-        <v>2.188</v>
+        <v>0.859</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C121">
-        <v>2.934</v>
+        <v>0.159</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B122">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C122">
-        <v>2.935</v>
+        <v>0.039</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B123">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C123">
-        <v>2.897</v>
+        <v>0.033</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B124">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C124">
-        <v>2.476</v>
+        <v>0.033</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45752</v>
+        <v>45757</v>
       </c>
       <c r="B125">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C125">
-        <v>2.079</v>
+        <v>0.033</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B126">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C126">
-        <v>1.684</v>
+        <v>0.033</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B127">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C127">
-        <v>0.957</v>
+        <v>0.033</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B128">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C128">
-        <v>0.444</v>
+        <v>0.033</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C129">
-        <v>0.082</v>
+        <v>0.033</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B130">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C130">
         <v>0.033</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B131">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C131">
         <v>0.033</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B132">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C132">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B133">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C133">
-        <v>0.033</v>
+        <v>0.158</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C134">
-        <v>0.033</v>
+        <v>0.854</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C135">
-        <v>0.033</v>
+        <v>1.755</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C136">
-        <v>0.033</v>
+        <v>2.377</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B137">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C137">
-        <v>0.033</v>
+        <v>3.051</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C138">
-        <v>0.033</v>
+        <v>3.221</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B139">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C139">
-        <v>0.033</v>
+        <v>3.371</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B140">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C140">
-        <v>0.033</v>
+        <v>3.156</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B141">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C141">
-        <v>0.139</v>
+        <v>3.008</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C142">
-        <v>0.803</v>
+        <v>2.297</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B143">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C143">
-        <v>1.748</v>
+        <v>1.697</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C144">
-        <v>2.622</v>
+        <v>0.829</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B145">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C145">
-        <v>3.131</v>
+        <v>0.155</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B146">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C146">
-        <v>3.564</v>
+        <v>0.033</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B147">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C147">
-        <v>3.517</v>
+        <v>0.033</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B148">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C148">
-        <v>2.976</v>
+        <v>0.033</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B149">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C149">
-        <v>2.451</v>
+        <v>0.033</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B150">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C150">
-        <v>1.854</v>
+        <v>0.033</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B151">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C151">
-        <v>1.405</v>
+        <v>0.033</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B152">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C152">
-        <v>0.67</v>
+        <v>0.033</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B153">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C153">
-        <v>0.127</v>
+        <v>0.033</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B154">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C154">
-        <v>0.043</v>
+        <v>0.033</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B155">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C155">
-        <v>0.039</v>
+        <v>0.033</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C156">
-        <v>0.039</v>
+        <v>0.033</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B157">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C157">
-        <v>0.034</v>
+        <v>0.227</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C158">
-        <v>0.033</v>
+        <v>0.919</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B159">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C159">
-        <v>0.033</v>
+        <v>2.062</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B160">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C160">
-        <v>0.033</v>
+        <v>3.451</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C161">
-        <v>0.033</v>
+        <v>4.402</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B162">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C162">
-        <v>0.033</v>
+        <v>4.586</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B163">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C163">
-        <v>0.033</v>
+        <v>4.587</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B164">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C164">
-        <v>0.033</v>
+        <v>4.295</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B165">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C165">
-        <v>0.08500000000000001</v>
+        <v>4.007</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B166">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C166">
-        <v>0.377</v>
+        <v>3.106</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B167">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C167">
-        <v>0.853</v>
+        <v>1.99</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B168">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C168">
-        <v>1.217</v>
+        <v>0.896</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B169">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C169">
-        <v>1.756</v>
+        <v>0.227</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B170">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C170">
-        <v>1.791</v>
+        <v>0.033</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding the Improved Wind Production Forecast model
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,405 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>05.04.202521</t>
-  </si>
-  <si>
-    <t>05.04.202522</t>
-  </si>
-  <si>
-    <t>05.04.202523</t>
-  </si>
-  <si>
-    <t>05.04.202524</t>
-  </si>
-  <si>
-    <t>06.04.20251</t>
-  </si>
-  <si>
-    <t>06.04.20252</t>
-  </si>
-  <si>
-    <t>06.04.20253</t>
-  </si>
-  <si>
-    <t>06.04.20254</t>
-  </si>
-  <si>
-    <t>06.04.20255</t>
-  </si>
-  <si>
-    <t>06.04.20256</t>
-  </si>
-  <si>
-    <t>06.04.20257</t>
-  </si>
-  <si>
-    <t>06.04.20258</t>
-  </si>
-  <si>
-    <t>06.04.20259</t>
-  </si>
-  <si>
-    <t>06.04.202510</t>
-  </si>
-  <si>
-    <t>06.04.202511</t>
-  </si>
-  <si>
-    <t>06.04.202512</t>
-  </si>
-  <si>
-    <t>06.04.202513</t>
-  </si>
-  <si>
-    <t>06.04.202514</t>
-  </si>
-  <si>
-    <t>06.04.202515</t>
-  </si>
-  <si>
-    <t>06.04.202516</t>
-  </si>
-  <si>
-    <t>06.04.202517</t>
-  </si>
-  <si>
-    <t>06.04.202518</t>
-  </si>
-  <si>
-    <t>06.04.202519</t>
-  </si>
-  <si>
-    <t>06.04.202520</t>
-  </si>
-  <si>
-    <t>06.04.202521</t>
-  </si>
-  <si>
-    <t>06.04.202522</t>
-  </si>
-  <si>
-    <t>06.04.202523</t>
-  </si>
-  <si>
-    <t>06.04.202524</t>
-  </si>
-  <si>
-    <t>07.04.20251</t>
-  </si>
-  <si>
-    <t>07.04.20252</t>
-  </si>
-  <si>
-    <t>07.04.20253</t>
-  </si>
-  <si>
-    <t>07.04.20254</t>
-  </si>
-  <si>
-    <t>07.04.20255</t>
-  </si>
-  <si>
-    <t>07.04.20256</t>
-  </si>
-  <si>
-    <t>07.04.20257</t>
-  </si>
-  <si>
-    <t>07.04.20258</t>
-  </si>
-  <si>
-    <t>07.04.20259</t>
-  </si>
-  <si>
-    <t>07.04.202510</t>
-  </si>
-  <si>
-    <t>07.04.202511</t>
-  </si>
-  <si>
-    <t>07.04.202512</t>
-  </si>
-  <si>
-    <t>07.04.202513</t>
-  </si>
-  <si>
-    <t>07.04.202514</t>
-  </si>
-  <si>
-    <t>07.04.202515</t>
-  </si>
-  <si>
-    <t>07.04.202516</t>
-  </si>
-  <si>
-    <t>07.04.202517</t>
-  </si>
-  <si>
-    <t>07.04.202518</t>
-  </si>
-  <si>
-    <t>07.04.202519</t>
-  </si>
-  <si>
-    <t>07.04.202520</t>
-  </si>
-  <si>
-    <t>07.04.202521</t>
-  </si>
-  <si>
-    <t>07.04.202522</t>
-  </si>
-  <si>
-    <t>07.04.202523</t>
-  </si>
-  <si>
-    <t>07.04.202524</t>
-  </si>
-  <si>
-    <t>08.04.20251</t>
-  </si>
-  <si>
-    <t>08.04.20252</t>
-  </si>
-  <si>
-    <t>08.04.20253</t>
-  </si>
-  <si>
-    <t>08.04.20254</t>
-  </si>
-  <si>
-    <t>08.04.20255</t>
-  </si>
-  <si>
-    <t>08.04.20256</t>
-  </si>
-  <si>
-    <t>08.04.20257</t>
-  </si>
-  <si>
-    <t>08.04.20258</t>
-  </si>
-  <si>
-    <t>08.04.20259</t>
-  </si>
-  <si>
-    <t>08.04.202510</t>
-  </si>
-  <si>
-    <t>08.04.202511</t>
-  </si>
-  <si>
-    <t>08.04.202512</t>
-  </si>
-  <si>
-    <t>08.04.202513</t>
-  </si>
-  <si>
-    <t>08.04.202514</t>
-  </si>
-  <si>
-    <t>08.04.202515</t>
-  </si>
-  <si>
-    <t>08.04.202516</t>
-  </si>
-  <si>
-    <t>08.04.202517</t>
-  </si>
-  <si>
-    <t>08.04.202518</t>
-  </si>
-  <si>
-    <t>08.04.202519</t>
-  </si>
-  <si>
-    <t>08.04.202520</t>
-  </si>
-  <si>
-    <t>08.04.202521</t>
-  </si>
-  <si>
-    <t>08.04.202522</t>
-  </si>
-  <si>
-    <t>08.04.202523</t>
-  </si>
-  <si>
-    <t>08.04.202524</t>
-  </si>
-  <si>
-    <t>09.04.20251</t>
-  </si>
-  <si>
-    <t>09.04.20252</t>
-  </si>
-  <si>
-    <t>09.04.20253</t>
-  </si>
-  <si>
-    <t>09.04.20254</t>
-  </si>
-  <si>
-    <t>09.04.20255</t>
-  </si>
-  <si>
-    <t>09.04.20256</t>
-  </si>
-  <si>
-    <t>09.04.20257</t>
-  </si>
-  <si>
-    <t>09.04.20258</t>
-  </si>
-  <si>
-    <t>09.04.20259</t>
-  </si>
-  <si>
-    <t>09.04.202510</t>
-  </si>
-  <si>
-    <t>09.04.202511</t>
-  </si>
-  <si>
-    <t>09.04.202512</t>
-  </si>
-  <si>
-    <t>09.04.202513</t>
-  </si>
-  <si>
-    <t>09.04.202514</t>
-  </si>
-  <si>
-    <t>09.04.202515</t>
-  </si>
-  <si>
-    <t>09.04.202516</t>
-  </si>
-  <si>
-    <t>09.04.202517</t>
-  </si>
-  <si>
-    <t>09.04.202518</t>
-  </si>
-  <si>
-    <t>09.04.202519</t>
-  </si>
-  <si>
-    <t>09.04.202520</t>
-  </si>
-  <si>
-    <t>09.04.202521</t>
-  </si>
-  <si>
-    <t>09.04.202522</t>
-  </si>
-  <si>
-    <t>09.04.202523</t>
-  </si>
-  <si>
-    <t>09.04.202524</t>
-  </si>
-  <si>
-    <t>10.04.20251</t>
-  </si>
-  <si>
-    <t>10.04.20252</t>
-  </si>
-  <si>
-    <t>10.04.20253</t>
-  </si>
-  <si>
-    <t>10.04.20254</t>
-  </si>
-  <si>
-    <t>10.04.20255</t>
-  </si>
-  <si>
-    <t>10.04.20256</t>
-  </si>
-  <si>
-    <t>10.04.20257</t>
-  </si>
-  <si>
-    <t>10.04.20258</t>
-  </si>
-  <si>
-    <t>10.04.20259</t>
-  </si>
-  <si>
-    <t>10.04.202510</t>
-  </si>
-  <si>
-    <t>10.04.202511</t>
-  </si>
-  <si>
-    <t>10.04.202512</t>
-  </si>
-  <si>
-    <t>10.04.202513</t>
-  </si>
-  <si>
-    <t>10.04.202514</t>
-  </si>
-  <si>
-    <t>10.04.202515</t>
-  </si>
-  <si>
-    <t>10.04.202516</t>
-  </si>
-  <si>
-    <t>10.04.202517</t>
-  </si>
-  <si>
-    <t>10.04.202518</t>
-  </si>
-  <si>
-    <t>10.04.202519</t>
-  </si>
-  <si>
-    <t>10.04.202520</t>
-  </si>
-  <si>
-    <t>10.04.202521</t>
-  </si>
-  <si>
-    <t>10.04.202522</t>
-  </si>
-  <si>
-    <t>10.04.202523</t>
-  </si>
-  <si>
-    <t>10.04.202524</t>
-  </si>
-  <si>
-    <t>11.04.20251</t>
-  </si>
-  <si>
-    <t>11.04.20252</t>
-  </si>
-  <si>
-    <t>11.04.20253</t>
-  </si>
-  <si>
-    <t>11.04.20254</t>
-  </si>
-  <si>
-    <t>11.04.20255</t>
-  </si>
-  <si>
-    <t>11.04.20256</t>
-  </si>
-  <si>
-    <t>11.04.20257</t>
-  </si>
-  <si>
-    <t>11.04.20258</t>
-  </si>
-  <si>
-    <t>11.04.20259</t>
-  </si>
-  <si>
     <t>11.04.202510</t>
   </si>
   <si>
@@ -533,6 +134,405 @@
   </si>
   <si>
     <t>12.04.202521</t>
+  </si>
+  <si>
+    <t>12.04.202522</t>
+  </si>
+  <si>
+    <t>12.04.202523</t>
+  </si>
+  <si>
+    <t>12.04.202524</t>
+  </si>
+  <si>
+    <t>13.04.20251</t>
+  </si>
+  <si>
+    <t>13.04.20252</t>
+  </si>
+  <si>
+    <t>13.04.20253</t>
+  </si>
+  <si>
+    <t>13.04.20254</t>
+  </si>
+  <si>
+    <t>13.04.20255</t>
+  </si>
+  <si>
+    <t>13.04.20256</t>
+  </si>
+  <si>
+    <t>13.04.20257</t>
+  </si>
+  <si>
+    <t>13.04.20258</t>
+  </si>
+  <si>
+    <t>13.04.20259</t>
+  </si>
+  <si>
+    <t>13.04.202510</t>
+  </si>
+  <si>
+    <t>13.04.202511</t>
+  </si>
+  <si>
+    <t>13.04.202512</t>
+  </si>
+  <si>
+    <t>13.04.202513</t>
+  </si>
+  <si>
+    <t>13.04.202514</t>
+  </si>
+  <si>
+    <t>13.04.202515</t>
+  </si>
+  <si>
+    <t>13.04.202516</t>
+  </si>
+  <si>
+    <t>13.04.202517</t>
+  </si>
+  <si>
+    <t>13.04.202518</t>
+  </si>
+  <si>
+    <t>13.04.202519</t>
+  </si>
+  <si>
+    <t>13.04.202520</t>
+  </si>
+  <si>
+    <t>13.04.202521</t>
+  </si>
+  <si>
+    <t>13.04.202522</t>
+  </si>
+  <si>
+    <t>13.04.202523</t>
+  </si>
+  <si>
+    <t>13.04.202524</t>
+  </si>
+  <si>
+    <t>14.04.20251</t>
+  </si>
+  <si>
+    <t>14.04.20252</t>
+  </si>
+  <si>
+    <t>14.04.20253</t>
+  </si>
+  <si>
+    <t>14.04.20254</t>
+  </si>
+  <si>
+    <t>14.04.20255</t>
+  </si>
+  <si>
+    <t>14.04.20256</t>
+  </si>
+  <si>
+    <t>14.04.20257</t>
+  </si>
+  <si>
+    <t>14.04.20258</t>
+  </si>
+  <si>
+    <t>14.04.20259</t>
+  </si>
+  <si>
+    <t>14.04.202510</t>
+  </si>
+  <si>
+    <t>14.04.202511</t>
+  </si>
+  <si>
+    <t>14.04.202512</t>
+  </si>
+  <si>
+    <t>14.04.202513</t>
+  </si>
+  <si>
+    <t>14.04.202514</t>
+  </si>
+  <si>
+    <t>14.04.202515</t>
+  </si>
+  <si>
+    <t>14.04.202516</t>
+  </si>
+  <si>
+    <t>14.04.202517</t>
+  </si>
+  <si>
+    <t>14.04.202518</t>
+  </si>
+  <si>
+    <t>14.04.202519</t>
+  </si>
+  <si>
+    <t>14.04.202520</t>
+  </si>
+  <si>
+    <t>14.04.202521</t>
+  </si>
+  <si>
+    <t>14.04.202522</t>
+  </si>
+  <si>
+    <t>14.04.202523</t>
+  </si>
+  <si>
+    <t>14.04.202524</t>
+  </si>
+  <si>
+    <t>15.04.20251</t>
+  </si>
+  <si>
+    <t>15.04.20252</t>
+  </si>
+  <si>
+    <t>15.04.20253</t>
+  </si>
+  <si>
+    <t>15.04.20254</t>
+  </si>
+  <si>
+    <t>15.04.20255</t>
+  </si>
+  <si>
+    <t>15.04.20256</t>
+  </si>
+  <si>
+    <t>15.04.20257</t>
+  </si>
+  <si>
+    <t>15.04.20258</t>
+  </si>
+  <si>
+    <t>15.04.20259</t>
+  </si>
+  <si>
+    <t>15.04.202510</t>
+  </si>
+  <si>
+    <t>15.04.202511</t>
+  </si>
+  <si>
+    <t>15.04.202512</t>
+  </si>
+  <si>
+    <t>15.04.202513</t>
+  </si>
+  <si>
+    <t>15.04.202514</t>
+  </si>
+  <si>
+    <t>15.04.202515</t>
+  </si>
+  <si>
+    <t>15.04.202516</t>
+  </si>
+  <si>
+    <t>15.04.202517</t>
+  </si>
+  <si>
+    <t>15.04.202518</t>
+  </si>
+  <si>
+    <t>15.04.202519</t>
+  </si>
+  <si>
+    <t>15.04.202520</t>
+  </si>
+  <si>
+    <t>15.04.202521</t>
+  </si>
+  <si>
+    <t>15.04.202522</t>
+  </si>
+  <si>
+    <t>15.04.202523</t>
+  </si>
+  <si>
+    <t>15.04.202524</t>
+  </si>
+  <si>
+    <t>16.04.20251</t>
+  </si>
+  <si>
+    <t>16.04.20252</t>
+  </si>
+  <si>
+    <t>16.04.20253</t>
+  </si>
+  <si>
+    <t>16.04.20254</t>
+  </si>
+  <si>
+    <t>16.04.20255</t>
+  </si>
+  <si>
+    <t>16.04.20256</t>
+  </si>
+  <si>
+    <t>16.04.20257</t>
+  </si>
+  <si>
+    <t>16.04.20258</t>
+  </si>
+  <si>
+    <t>16.04.20259</t>
+  </si>
+  <si>
+    <t>16.04.202510</t>
+  </si>
+  <si>
+    <t>16.04.202511</t>
+  </si>
+  <si>
+    <t>16.04.202512</t>
+  </si>
+  <si>
+    <t>16.04.202513</t>
+  </si>
+  <si>
+    <t>16.04.202514</t>
+  </si>
+  <si>
+    <t>16.04.202515</t>
+  </si>
+  <si>
+    <t>16.04.202516</t>
+  </si>
+  <si>
+    <t>16.04.202517</t>
+  </si>
+  <si>
+    <t>16.04.202518</t>
+  </si>
+  <si>
+    <t>16.04.202519</t>
+  </si>
+  <si>
+    <t>16.04.202520</t>
+  </si>
+  <si>
+    <t>16.04.202521</t>
+  </si>
+  <si>
+    <t>16.04.202522</t>
+  </si>
+  <si>
+    <t>16.04.202523</t>
+  </si>
+  <si>
+    <t>16.04.202524</t>
+  </si>
+  <si>
+    <t>17.04.20251</t>
+  </si>
+  <si>
+    <t>17.04.20252</t>
+  </si>
+  <si>
+    <t>17.04.20253</t>
+  </si>
+  <si>
+    <t>17.04.20254</t>
+  </si>
+  <si>
+    <t>17.04.20255</t>
+  </si>
+  <si>
+    <t>17.04.20256</t>
+  </si>
+  <si>
+    <t>17.04.20257</t>
+  </si>
+  <si>
+    <t>17.04.20258</t>
+  </si>
+  <si>
+    <t>17.04.20259</t>
+  </si>
+  <si>
+    <t>17.04.202510</t>
+  </si>
+  <si>
+    <t>17.04.202511</t>
+  </si>
+  <si>
+    <t>17.04.202512</t>
+  </si>
+  <si>
+    <t>17.04.202513</t>
+  </si>
+  <si>
+    <t>17.04.202514</t>
+  </si>
+  <si>
+    <t>17.04.202515</t>
+  </si>
+  <si>
+    <t>17.04.202516</t>
+  </si>
+  <si>
+    <t>17.04.202517</t>
+  </si>
+  <si>
+    <t>17.04.202518</t>
+  </si>
+  <si>
+    <t>17.04.202519</t>
+  </si>
+  <si>
+    <t>17.04.202520</t>
+  </si>
+  <si>
+    <t>17.04.202521</t>
+  </si>
+  <si>
+    <t>17.04.202522</t>
+  </si>
+  <si>
+    <t>17.04.202523</t>
+  </si>
+  <si>
+    <t>17.04.202524</t>
+  </si>
+  <si>
+    <t>18.04.20251</t>
+  </si>
+  <si>
+    <t>18.04.20252</t>
+  </si>
+  <si>
+    <t>18.04.20253</t>
+  </si>
+  <si>
+    <t>18.04.20254</t>
+  </si>
+  <si>
+    <t>18.04.20255</t>
+  </si>
+  <si>
+    <t>18.04.20256</t>
+  </si>
+  <si>
+    <t>18.04.20257</t>
+  </si>
+  <si>
+    <t>18.04.20258</t>
+  </si>
+  <si>
+    <t>18.04.20259</t>
+  </si>
+  <si>
+    <t>18.04.202510</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.045</v>
+        <v>0.066</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0.045</v>
+        <v>0.066</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0.033</v>
+        <v>2.066</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45752</v>
+        <v>45758</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0.033</v>
+        <v>2.857</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0.033</v>
+        <v>3.608</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0.033</v>
+        <v>3.744</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.033</v>
+        <v>3.437</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0.033</v>
+        <v>2.765</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0.034</v>
+        <v>1.68</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0.034</v>
+        <v>0.734</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0.035</v>
+        <v>0.146</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>0.217</v>
+        <v>0.033</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>1.113</v>
+        <v>0.033</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>2.72</v>
+        <v>0.033</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45753</v>
+        <v>45758</v>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C16">
-        <v>4.04</v>
+        <v>0.033</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>4.288</v>
+        <v>0.033</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B18">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>4.284</v>
+        <v>0.033</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>4.087</v>
+        <v>0.033</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B20">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>3.574</v>
+        <v>0.033</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B21">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>3.329</v>
+        <v>0.034</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B22">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>2.895</v>
+        <v>0.034</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B23">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>2.044</v>
+        <v>0.034</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B24">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>0.894</v>
+        <v>0.255</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B25">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>0.223</v>
+        <v>1.331</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B26">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0.039</v>
+        <v>2.347</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B27">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>0.033</v>
+        <v>3.475</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B28">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>0.033</v>
+        <v>3.95</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45753</v>
+        <v>45759</v>
       </c>
       <c r="B29">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>0.033</v>
+        <v>4.04</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0.034</v>
+        <v>3.961</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0.034</v>
+        <v>3.734</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0.035</v>
+        <v>3.372</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0.036</v>
+        <v>2.943</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0.035</v>
+        <v>1.789</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0.034</v>
+        <v>0.91</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>0.034</v>
+        <v>0.227</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>0.218</v>
+        <v>0.033</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B38">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C38">
-        <v>1.014</v>
+        <v>0.033</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B39">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>2.114</v>
+        <v>0.033</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45754</v>
+        <v>45759</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C40">
-        <v>3.116</v>
+        <v>0.033</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>3.625</v>
+        <v>0.034</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B42">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>3.841</v>
+        <v>0.034</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B43">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>3.838</v>
+        <v>0.034</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B44">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>3.474</v>
+        <v>0.034</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B45">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>2.964</v>
+        <v>0.034</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B46">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>2.189</v>
+        <v>0.034</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B47">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>1.512</v>
+        <v>0.034</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B48">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>0.636</v>
+        <v>0.276</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B49">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0.099</v>
+        <v>1.067</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B50">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>0.042</v>
+        <v>2.11</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B51">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>0.041</v>
+        <v>3.058</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B52">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>0.039</v>
+        <v>3.853</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45754</v>
+        <v>45760</v>
       </c>
       <c r="B53">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>0.039</v>
+        <v>4.096</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>0.036</v>
+        <v>4.161</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0.036</v>
+        <v>4.033</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0.036</v>
+        <v>3.855</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0.036</v>
+        <v>3.332</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0.036</v>
+        <v>2.29</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0.036</v>
+        <v>1.257</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B60">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0.036</v>
+        <v>0.251</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B61">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>0.158</v>
+        <v>0.033</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B62">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C62">
-        <v>0.915</v>
+        <v>0.033</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C63">
-        <v>1.862</v>
+        <v>0.033</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45755</v>
+        <v>45760</v>
       </c>
       <c r="B64">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>3.022</v>
+        <v>0.033</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B65">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>3.824</v>
+        <v>0.034</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B66">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>4.016</v>
+        <v>0.033</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B67">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>4.067</v>
+        <v>0.033</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B68">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>3.937</v>
+        <v>0.033</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B69">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>3.655</v>
+        <v>0.033</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B70">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>2.892</v>
+        <v>0.033</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B71">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>1.73</v>
+        <v>0.033</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B72">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>0.786</v>
+        <v>0.098</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B73">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>0.152</v>
+        <v>0.377</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B74">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>0.039</v>
+        <v>0.887</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B75">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>0.039</v>
+        <v>1.526</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B76">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>0.034</v>
+        <v>1.782</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45755</v>
+        <v>45761</v>
       </c>
       <c r="B77">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>0.033</v>
+        <v>2.024</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>0.033</v>
+        <v>2.35</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0.034</v>
+        <v>2.792</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0.034</v>
+        <v>2.474</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0.034</v>
+        <v>1.986</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B82">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0.034</v>
+        <v>1.621</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B83">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C83">
-        <v>0.034</v>
+        <v>0.755</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B84">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>0.034</v>
+        <v>0.159</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B85">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C85">
-        <v>0.222</v>
+        <v>0.033</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B86">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C86">
-        <v>1.014</v>
+        <v>0.033</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B87">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C87">
-        <v>2.31</v>
+        <v>0.033</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45756</v>
+        <v>45761</v>
       </c>
       <c r="B88">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C88">
-        <v>3.496</v>
+        <v>0.033</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B89">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>4.57</v>
+        <v>0.033</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B90">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>4.437</v>
+        <v>0.033</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B91">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>4.306</v>
+        <v>0.033</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B92">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>3.731</v>
+        <v>0.033</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B93">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>3.074</v>
+        <v>0.035</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B94">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>2.393</v>
+        <v>0.033</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B95">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>1.675</v>
+        <v>0.033</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B96">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>0.764</v>
+        <v>0.139</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B97">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>0.152</v>
+        <v>0.371</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B98">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>0.039</v>
+        <v>0.775</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B99">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>0.033</v>
+        <v>1.073</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B100">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>0.033</v>
+        <v>1.551</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45756</v>
+        <v>45762</v>
       </c>
       <c r="B101">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>0.033</v>
+        <v>1.732</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>0.033</v>
+        <v>1.754</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>0.033</v>
+        <v>1.715</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>0.033</v>
+        <v>1.676</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0.033</v>
+        <v>1.527</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>0.033</v>
+        <v>1.051</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B107">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0.033</v>
+        <v>0.657</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C108">
-        <v>0.033</v>
+        <v>0.155</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B109">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C109">
-        <v>0.154</v>
+        <v>0.033</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B110">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C110">
-        <v>0.75</v>
+        <v>0.033</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B111">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C111">
-        <v>1.657</v>
+        <v>0.033</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45757</v>
+        <v>45762</v>
       </c>
       <c r="B112">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C112">
-        <v>2.19</v>
+        <v>0.033</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B113">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>2.877</v>
+        <v>0.033</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B114">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>3.006</v>
+        <v>0.033</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B115">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>3.127</v>
+        <v>0.033</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B116">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>3.006</v>
+        <v>0.033</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B117">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>2.863</v>
+        <v>0.033</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B118">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>2.356</v>
+        <v>0.033</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B119">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>1.726</v>
+        <v>0.033</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B120">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>0.859</v>
+        <v>0.139</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B121">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>0.159</v>
+        <v>0.372</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B122">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>0.039</v>
+        <v>0.851</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B123">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>0.033</v>
+        <v>1.178</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B124">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>0.033</v>
+        <v>1.681</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45757</v>
+        <v>45763</v>
       </c>
       <c r="B125">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>0.033</v>
+        <v>1.86</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>0.033</v>
+        <v>2.462</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>0.033</v>
+        <v>2.959</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B128">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>0.033</v>
+        <v>2.929</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B129">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>0.033</v>
+        <v>2.256</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B130">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>0.033</v>
+        <v>1.662</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B131">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0.033</v>
+        <v>0.886</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B132">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0.035</v>
+        <v>0.232</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B133">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C133">
-        <v>0.158</v>
+        <v>0.033</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B134">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C134">
-        <v>0.854</v>
+        <v>0.033</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B135">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C135">
-        <v>1.755</v>
+        <v>0.033</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45758</v>
+        <v>45763</v>
       </c>
       <c r="B136">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C136">
-        <v>2.377</v>
+        <v>0.033</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B137">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C137">
-        <v>3.051</v>
+        <v>0.033</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B138">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>3.221</v>
+        <v>0.033</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B139">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>3.371</v>
+        <v>0.033</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B140">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>3.156</v>
+        <v>0.035</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B141">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>3.008</v>
+        <v>0.035</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B142">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>2.297</v>
+        <v>0.036</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B143">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>1.697</v>
+        <v>0.035</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B144">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>0.829</v>
+        <v>0.284</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B145">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>0.155</v>
+        <v>1.009</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B146">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>0.033</v>
+        <v>2.096</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B147">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>0.033</v>
+        <v>3.09</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B148">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>0.033</v>
+        <v>3.712</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45758</v>
+        <v>45764</v>
       </c>
       <c r="B149">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>0.033</v>
+        <v>4.288</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>0.033</v>
+        <v>4.266</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B151">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>0.033</v>
+        <v>4.116</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B152">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>0.033</v>
+        <v>4.107</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B153">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>0.033</v>
+        <v>3.456</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B154">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C154">
-        <v>0.033</v>
+        <v>2.576</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B155">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0.033</v>
+        <v>1.4</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B156">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C156">
-        <v>0.033</v>
+        <v>0.303</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B157">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>0.227</v>
+        <v>0.033</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B158">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C158">
-        <v>0.919</v>
+        <v>0.033</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B159">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C159">
-        <v>2.062</v>
+        <v>0.033</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45759</v>
+        <v>45764</v>
       </c>
       <c r="B160">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C160">
-        <v>3.451</v>
+        <v>0.033</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B161">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C161">
-        <v>4.402</v>
+        <v>0.034</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B162">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>4.586</v>
+        <v>0.034</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B163">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>4.587</v>
+        <v>0.033</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B164">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>4.295</v>
+        <v>0.033</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B165">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>4.007</v>
+        <v>0.033</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B166">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>3.106</v>
+        <v>0.033</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B167">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>1.99</v>
+        <v>0.033</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B168">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>0.896</v>
+        <v>0.28</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B169">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>0.227</v>
+        <v>0.957</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45759</v>
+        <v>45765</v>
       </c>
       <c r="B170">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>0.033</v>
+        <v>1.805</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retraining the production models for Kahraman
</commit_message>
<xml_diff>
--- a/Kahraman/Results_Production_Kahraman_xgb.xlsx
+++ b/Kahraman/Results_Production_Kahraman_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>07.05.202511</t>
-  </si>
-  <si>
-    <t>07.05.202512</t>
-  </si>
-  <si>
-    <t>07.05.202513</t>
-  </si>
-  <si>
-    <t>07.05.202514</t>
-  </si>
-  <si>
-    <t>07.05.202515</t>
-  </si>
-  <si>
-    <t>07.05.202516</t>
-  </si>
-  <si>
-    <t>07.05.202517</t>
-  </si>
-  <si>
-    <t>07.05.202518</t>
-  </si>
-  <si>
-    <t>07.05.202519</t>
-  </si>
-  <si>
-    <t>07.05.202520</t>
-  </si>
-  <si>
-    <t>07.05.202521</t>
-  </si>
-  <si>
-    <t>07.05.202522</t>
-  </si>
-  <si>
-    <t>07.05.202523</t>
-  </si>
-  <si>
-    <t>07.05.202524</t>
-  </si>
-  <si>
-    <t>08.05.20251</t>
-  </si>
-  <si>
-    <t>08.05.20252</t>
-  </si>
-  <si>
-    <t>08.05.20253</t>
-  </si>
-  <si>
-    <t>08.05.20254</t>
-  </si>
-  <si>
-    <t>08.05.20255</t>
-  </si>
-  <si>
-    <t>08.05.20256</t>
-  </si>
-  <si>
-    <t>08.05.20257</t>
-  </si>
-  <si>
-    <t>08.05.20258</t>
-  </si>
-  <si>
-    <t>08.05.20259</t>
-  </si>
-  <si>
-    <t>08.05.202510</t>
-  </si>
-  <si>
-    <t>08.05.202511</t>
-  </si>
-  <si>
-    <t>08.05.202512</t>
-  </si>
-  <si>
-    <t>08.05.202513</t>
-  </si>
-  <si>
-    <t>08.05.202514</t>
-  </si>
-  <si>
-    <t>08.05.202515</t>
-  </si>
-  <si>
-    <t>08.05.202516</t>
-  </si>
-  <si>
-    <t>08.05.202517</t>
-  </si>
-  <si>
-    <t>08.05.202518</t>
-  </si>
-  <si>
-    <t>08.05.202519</t>
-  </si>
-  <si>
-    <t>08.05.202520</t>
-  </si>
-  <si>
-    <t>08.05.202521</t>
-  </si>
-  <si>
-    <t>08.05.202522</t>
-  </si>
-  <si>
-    <t>08.05.202523</t>
-  </si>
-  <si>
-    <t>08.05.202524</t>
-  </si>
-  <si>
-    <t>09.05.20251</t>
-  </si>
-  <si>
-    <t>09.05.20252</t>
-  </si>
-  <si>
-    <t>09.05.20253</t>
-  </si>
-  <si>
-    <t>09.05.20254</t>
-  </si>
-  <si>
-    <t>09.05.20255</t>
-  </si>
-  <si>
-    <t>09.05.20256</t>
-  </si>
-  <si>
-    <t>09.05.20257</t>
-  </si>
-  <si>
-    <t>09.05.20258</t>
-  </si>
-  <si>
-    <t>09.05.20259</t>
-  </si>
-  <si>
-    <t>09.05.202510</t>
-  </si>
-  <si>
-    <t>09.05.202511</t>
-  </si>
-  <si>
-    <t>09.05.202512</t>
-  </si>
-  <si>
-    <t>09.05.202513</t>
-  </si>
-  <si>
-    <t>09.05.202514</t>
-  </si>
-  <si>
-    <t>09.05.202515</t>
-  </si>
-  <si>
-    <t>09.05.202516</t>
-  </si>
-  <si>
-    <t>09.05.202517</t>
-  </si>
-  <si>
-    <t>09.05.202518</t>
-  </si>
-  <si>
-    <t>09.05.202519</t>
-  </si>
-  <si>
-    <t>09.05.202520</t>
-  </si>
-  <si>
-    <t>09.05.202521</t>
-  </si>
-  <si>
-    <t>09.05.202522</t>
-  </si>
-  <si>
-    <t>09.05.202523</t>
-  </si>
-  <si>
-    <t>09.05.202524</t>
-  </si>
-  <si>
-    <t>10.05.20251</t>
-  </si>
-  <si>
-    <t>10.05.20252</t>
-  </si>
-  <si>
-    <t>10.05.20253</t>
-  </si>
-  <si>
-    <t>10.05.20254</t>
-  </si>
-  <si>
-    <t>10.05.20255</t>
-  </si>
-  <si>
-    <t>10.05.20256</t>
-  </si>
-  <si>
-    <t>10.05.20257</t>
-  </si>
-  <si>
-    <t>10.05.20258</t>
-  </si>
-  <si>
-    <t>10.05.20259</t>
-  </si>
-  <si>
-    <t>10.05.202510</t>
-  </si>
-  <si>
-    <t>10.05.202511</t>
-  </si>
-  <si>
-    <t>10.05.202512</t>
-  </si>
-  <si>
-    <t>10.05.202513</t>
-  </si>
-  <si>
-    <t>10.05.202514</t>
-  </si>
-  <si>
-    <t>10.05.202515</t>
-  </si>
-  <si>
-    <t>10.05.202516</t>
-  </si>
-  <si>
-    <t>10.05.202517</t>
-  </si>
-  <si>
-    <t>10.05.202518</t>
-  </si>
-  <si>
-    <t>10.05.202519</t>
-  </si>
-  <si>
-    <t>10.05.202520</t>
-  </si>
-  <si>
-    <t>10.05.202521</t>
-  </si>
-  <si>
-    <t>10.05.202522</t>
-  </si>
-  <si>
-    <t>10.05.202523</t>
-  </si>
-  <si>
-    <t>10.05.202524</t>
-  </si>
-  <si>
-    <t>11.05.20251</t>
-  </si>
-  <si>
-    <t>11.05.20252</t>
-  </si>
-  <si>
-    <t>11.05.20253</t>
-  </si>
-  <si>
-    <t>11.05.20254</t>
-  </si>
-  <si>
-    <t>11.05.20255</t>
-  </si>
-  <si>
-    <t>11.05.20256</t>
-  </si>
-  <si>
-    <t>11.05.20257</t>
-  </si>
-  <si>
-    <t>11.05.20258</t>
-  </si>
-  <si>
-    <t>11.05.20259</t>
-  </si>
-  <si>
-    <t>11.05.202510</t>
-  </si>
-  <si>
-    <t>11.05.202511</t>
-  </si>
-  <si>
-    <t>11.05.202512</t>
-  </si>
-  <si>
-    <t>11.05.202513</t>
-  </si>
-  <si>
-    <t>11.05.202514</t>
-  </si>
-  <si>
-    <t>11.05.202515</t>
-  </si>
-  <si>
-    <t>11.05.202516</t>
-  </si>
-  <si>
-    <t>11.05.202517</t>
-  </si>
-  <si>
-    <t>11.05.202518</t>
-  </si>
-  <si>
-    <t>11.05.202519</t>
-  </si>
-  <si>
-    <t>11.05.202520</t>
-  </si>
-  <si>
-    <t>11.05.202521</t>
-  </si>
-  <si>
-    <t>11.05.202522</t>
-  </si>
-  <si>
-    <t>11.05.202523</t>
-  </si>
-  <si>
-    <t>11.05.202524</t>
-  </si>
-  <si>
-    <t>12.05.20251</t>
-  </si>
-  <si>
-    <t>12.05.20252</t>
-  </si>
-  <si>
-    <t>12.05.20253</t>
-  </si>
-  <si>
-    <t>12.05.20254</t>
-  </si>
-  <si>
-    <t>12.05.20255</t>
-  </si>
-  <si>
-    <t>12.05.20256</t>
-  </si>
-  <si>
-    <t>12.05.20257</t>
-  </si>
-  <si>
-    <t>12.05.20258</t>
-  </si>
-  <si>
-    <t>12.05.20259</t>
-  </si>
-  <si>
-    <t>12.05.202510</t>
-  </si>
-  <si>
-    <t>12.05.202511</t>
-  </si>
-  <si>
-    <t>12.05.202512</t>
-  </si>
-  <si>
-    <t>12.05.202513</t>
-  </si>
-  <si>
-    <t>12.05.202514</t>
-  </si>
-  <si>
-    <t>12.05.202515</t>
-  </si>
-  <si>
-    <t>12.05.202516</t>
-  </si>
-  <si>
-    <t>12.05.202517</t>
-  </si>
-  <si>
-    <t>12.05.202518</t>
-  </si>
-  <si>
-    <t>12.05.202519</t>
-  </si>
-  <si>
-    <t>12.05.202520</t>
-  </si>
-  <si>
-    <t>12.05.202521</t>
-  </si>
-  <si>
-    <t>12.05.202522</t>
-  </si>
-  <si>
-    <t>12.05.202523</t>
-  </si>
-  <si>
-    <t>12.05.202524</t>
-  </si>
-  <si>
-    <t>13.05.20251</t>
-  </si>
-  <si>
-    <t>13.05.20252</t>
-  </si>
-  <si>
-    <t>13.05.20253</t>
-  </si>
-  <si>
-    <t>13.05.20254</t>
-  </si>
-  <si>
-    <t>13.05.20255</t>
-  </si>
-  <si>
-    <t>13.05.20256</t>
-  </si>
-  <si>
-    <t>13.05.20257</t>
-  </si>
-  <si>
-    <t>13.05.20258</t>
-  </si>
-  <si>
-    <t>13.05.20259</t>
-  </si>
-  <si>
-    <t>13.05.202510</t>
-  </si>
-  <si>
-    <t>13.05.202511</t>
-  </si>
-  <si>
-    <t>13.05.202512</t>
-  </si>
-  <si>
-    <t>13.05.202513</t>
-  </si>
-  <si>
-    <t>13.05.202514</t>
-  </si>
-  <si>
-    <t>13.05.202515</t>
-  </si>
-  <si>
-    <t>13.05.202516</t>
-  </si>
-  <si>
-    <t>13.05.202517</t>
-  </si>
-  <si>
-    <t>13.05.202518</t>
-  </si>
-  <si>
-    <t>13.05.202519</t>
-  </si>
-  <si>
-    <t>13.05.202520</t>
-  </si>
-  <si>
-    <t>13.05.202521</t>
-  </si>
-  <si>
-    <t>13.05.202522</t>
-  </si>
-  <si>
-    <t>13.05.202523</t>
-  </si>
-  <si>
-    <t>13.05.202524</t>
-  </si>
-  <si>
-    <t>14.05.20251</t>
-  </si>
-  <si>
-    <t>14.05.20252</t>
-  </si>
-  <si>
-    <t>14.05.20253</t>
-  </si>
-  <si>
-    <t>14.05.20254</t>
-  </si>
-  <si>
-    <t>14.05.20255</t>
-  </si>
-  <si>
-    <t>14.05.20256</t>
-  </si>
-  <si>
-    <t>14.05.20257</t>
-  </si>
-  <si>
-    <t>14.05.20258</t>
-  </si>
-  <si>
-    <t>14.05.20259</t>
-  </si>
-  <si>
-    <t>14.05.202510</t>
-  </si>
-  <si>
-    <t>14.05.202511</t>
+    <t>21.05.202510</t>
+  </si>
+  <si>
+    <t>21.05.202511</t>
+  </si>
+  <si>
+    <t>21.05.202512</t>
+  </si>
+  <si>
+    <t>21.05.202513</t>
+  </si>
+  <si>
+    <t>21.05.202514</t>
+  </si>
+  <si>
+    <t>21.05.202515</t>
+  </si>
+  <si>
+    <t>21.05.202516</t>
+  </si>
+  <si>
+    <t>21.05.202517</t>
+  </si>
+  <si>
+    <t>21.05.202518</t>
+  </si>
+  <si>
+    <t>21.05.202519</t>
+  </si>
+  <si>
+    <t>21.05.202520</t>
+  </si>
+  <si>
+    <t>21.05.202521</t>
+  </si>
+  <si>
+    <t>21.05.202522</t>
+  </si>
+  <si>
+    <t>21.05.202523</t>
+  </si>
+  <si>
+    <t>21.05.202524</t>
+  </si>
+  <si>
+    <t>22.05.20251</t>
+  </si>
+  <si>
+    <t>22.05.20252</t>
+  </si>
+  <si>
+    <t>22.05.20253</t>
+  </si>
+  <si>
+    <t>22.05.20254</t>
+  </si>
+  <si>
+    <t>22.05.20255</t>
+  </si>
+  <si>
+    <t>22.05.20256</t>
+  </si>
+  <si>
+    <t>22.05.20257</t>
+  </si>
+  <si>
+    <t>22.05.20258</t>
+  </si>
+  <si>
+    <t>22.05.20259</t>
+  </si>
+  <si>
+    <t>22.05.202510</t>
+  </si>
+  <si>
+    <t>22.05.202511</t>
+  </si>
+  <si>
+    <t>22.05.202512</t>
+  </si>
+  <si>
+    <t>22.05.202513</t>
+  </si>
+  <si>
+    <t>22.05.202514</t>
+  </si>
+  <si>
+    <t>22.05.202515</t>
+  </si>
+  <si>
+    <t>22.05.202516</t>
+  </si>
+  <si>
+    <t>22.05.202517</t>
+  </si>
+  <si>
+    <t>22.05.202518</t>
+  </si>
+  <si>
+    <t>22.05.202519</t>
+  </si>
+  <si>
+    <t>22.05.202520</t>
+  </si>
+  <si>
+    <t>22.05.202521</t>
+  </si>
+  <si>
+    <t>22.05.202522</t>
+  </si>
+  <si>
+    <t>22.05.202523</t>
+  </si>
+  <si>
+    <t>22.05.202524</t>
+  </si>
+  <si>
+    <t>23.05.20251</t>
+  </si>
+  <si>
+    <t>23.05.20252</t>
+  </si>
+  <si>
+    <t>23.05.20253</t>
+  </si>
+  <si>
+    <t>23.05.20254</t>
+  </si>
+  <si>
+    <t>23.05.20255</t>
+  </si>
+  <si>
+    <t>23.05.20256</t>
+  </si>
+  <si>
+    <t>23.05.20257</t>
+  </si>
+  <si>
+    <t>23.05.20258</t>
+  </si>
+  <si>
+    <t>23.05.20259</t>
+  </si>
+  <si>
+    <t>23.05.202510</t>
+  </si>
+  <si>
+    <t>23.05.202511</t>
+  </si>
+  <si>
+    <t>23.05.202512</t>
+  </si>
+  <si>
+    <t>23.05.202513</t>
+  </si>
+  <si>
+    <t>23.05.202514</t>
+  </si>
+  <si>
+    <t>23.05.202515</t>
+  </si>
+  <si>
+    <t>23.05.202516</t>
+  </si>
+  <si>
+    <t>23.05.202517</t>
+  </si>
+  <si>
+    <t>23.05.202518</t>
+  </si>
+  <si>
+    <t>23.05.202519</t>
+  </si>
+  <si>
+    <t>23.05.202520</t>
+  </si>
+  <si>
+    <t>23.05.202521</t>
+  </si>
+  <si>
+    <t>23.05.202522</t>
+  </si>
+  <si>
+    <t>23.05.202523</t>
+  </si>
+  <si>
+    <t>23.05.202524</t>
+  </si>
+  <si>
+    <t>24.05.20251</t>
+  </si>
+  <si>
+    <t>24.05.20252</t>
+  </si>
+  <si>
+    <t>24.05.20253</t>
+  </si>
+  <si>
+    <t>24.05.20254</t>
+  </si>
+  <si>
+    <t>24.05.20255</t>
+  </si>
+  <si>
+    <t>24.05.20256</t>
+  </si>
+  <si>
+    <t>24.05.20257</t>
+  </si>
+  <si>
+    <t>24.05.20258</t>
+  </si>
+  <si>
+    <t>24.05.20259</t>
+  </si>
+  <si>
+    <t>24.05.202510</t>
+  </si>
+  <si>
+    <t>24.05.202511</t>
+  </si>
+  <si>
+    <t>24.05.202512</t>
+  </si>
+  <si>
+    <t>24.05.202513</t>
+  </si>
+  <si>
+    <t>24.05.202514</t>
+  </si>
+  <si>
+    <t>24.05.202515</t>
+  </si>
+  <si>
+    <t>24.05.202516</t>
+  </si>
+  <si>
+    <t>24.05.202517</t>
+  </si>
+  <si>
+    <t>24.05.202518</t>
+  </si>
+  <si>
+    <t>24.05.202519</t>
+  </si>
+  <si>
+    <t>24.05.202520</t>
+  </si>
+  <si>
+    <t>24.05.202521</t>
+  </si>
+  <si>
+    <t>24.05.202522</t>
+  </si>
+  <si>
+    <t>24.05.202523</t>
+  </si>
+  <si>
+    <t>24.05.202524</t>
+  </si>
+  <si>
+    <t>25.05.20251</t>
+  </si>
+  <si>
+    <t>25.05.20252</t>
+  </si>
+  <si>
+    <t>25.05.20253</t>
+  </si>
+  <si>
+    <t>25.05.20254</t>
+  </si>
+  <si>
+    <t>25.05.20255</t>
+  </si>
+  <si>
+    <t>25.05.20256</t>
+  </si>
+  <si>
+    <t>25.05.20257</t>
+  </si>
+  <si>
+    <t>25.05.20258</t>
+  </si>
+  <si>
+    <t>25.05.20259</t>
+  </si>
+  <si>
+    <t>25.05.202510</t>
+  </si>
+  <si>
+    <t>25.05.202511</t>
+  </si>
+  <si>
+    <t>25.05.202512</t>
+  </si>
+  <si>
+    <t>25.05.202513</t>
+  </si>
+  <si>
+    <t>25.05.202514</t>
+  </si>
+  <si>
+    <t>25.05.202515</t>
+  </si>
+  <si>
+    <t>25.05.202516</t>
+  </si>
+  <si>
+    <t>25.05.202517</t>
+  </si>
+  <si>
+    <t>25.05.202518</t>
+  </si>
+  <si>
+    <t>25.05.202519</t>
+  </si>
+  <si>
+    <t>25.05.202520</t>
+  </si>
+  <si>
+    <t>25.05.202521</t>
+  </si>
+  <si>
+    <t>25.05.202522</t>
+  </si>
+  <si>
+    <t>25.05.202523</t>
+  </si>
+  <si>
+    <t>25.05.202524</t>
+  </si>
+  <si>
+    <t>26.05.20251</t>
+  </si>
+  <si>
+    <t>26.05.20252</t>
+  </si>
+  <si>
+    <t>26.05.20253</t>
+  </si>
+  <si>
+    <t>26.05.20254</t>
+  </si>
+  <si>
+    <t>26.05.20255</t>
+  </si>
+  <si>
+    <t>26.05.20256</t>
+  </si>
+  <si>
+    <t>26.05.20257</t>
+  </si>
+  <si>
+    <t>26.05.20258</t>
+  </si>
+  <si>
+    <t>26.05.20259</t>
+  </si>
+  <si>
+    <t>26.05.202510</t>
+  </si>
+  <si>
+    <t>26.05.202511</t>
+  </si>
+  <si>
+    <t>26.05.202512</t>
+  </si>
+  <si>
+    <t>26.05.202513</t>
+  </si>
+  <si>
+    <t>26.05.202514</t>
+  </si>
+  <si>
+    <t>26.05.202515</t>
+  </si>
+  <si>
+    <t>26.05.202516</t>
+  </si>
+  <si>
+    <t>26.05.202517</t>
+  </si>
+  <si>
+    <t>26.05.202518</t>
+  </si>
+  <si>
+    <t>26.05.202519</t>
+  </si>
+  <si>
+    <t>26.05.202520</t>
+  </si>
+  <si>
+    <t>26.05.202521</t>
+  </si>
+  <si>
+    <t>26.05.202522</t>
+  </si>
+  <si>
+    <t>26.05.202523</t>
+  </si>
+  <si>
+    <t>26.05.202524</t>
+  </si>
+  <si>
+    <t>27.05.20251</t>
+  </si>
+  <si>
+    <t>27.05.20252</t>
+  </si>
+  <si>
+    <t>27.05.20253</t>
+  </si>
+  <si>
+    <t>27.05.20254</t>
+  </si>
+  <si>
+    <t>27.05.20255</t>
+  </si>
+  <si>
+    <t>27.05.20256</t>
+  </si>
+  <si>
+    <t>27.05.20257</t>
+  </si>
+  <si>
+    <t>27.05.20258</t>
+  </si>
+  <si>
+    <t>27.05.20259</t>
+  </si>
+  <si>
+    <t>27.05.202510</t>
+  </si>
+  <si>
+    <t>27.05.202511</t>
+  </si>
+  <si>
+    <t>27.05.202512</t>
+  </si>
+  <si>
+    <t>27.05.202513</t>
+  </si>
+  <si>
+    <t>27.05.202514</t>
+  </si>
+  <si>
+    <t>27.05.202515</t>
+  </si>
+  <si>
+    <t>27.05.202516</t>
+  </si>
+  <si>
+    <t>27.05.202517</t>
+  </si>
+  <si>
+    <t>27.05.202518</t>
+  </si>
+  <si>
+    <t>27.05.202519</t>
+  </si>
+  <si>
+    <t>27.05.202520</t>
+  </si>
+  <si>
+    <t>27.05.202521</t>
+  </si>
+  <si>
+    <t>27.05.202522</t>
+  </si>
+  <si>
+    <t>27.05.202523</t>
+  </si>
+  <si>
+    <t>27.05.202524</t>
+  </si>
+  <si>
+    <t>28.05.20251</t>
+  </si>
+  <si>
+    <t>28.05.20252</t>
+  </si>
+  <si>
+    <t>28.05.20253</t>
+  </si>
+  <si>
+    <t>28.05.20254</t>
+  </si>
+  <si>
+    <t>28.05.20255</t>
+  </si>
+  <si>
+    <t>28.05.20256</t>
+  </si>
+  <si>
+    <t>28.05.20257</t>
+  </si>
+  <si>
+    <t>28.05.20258</t>
+  </si>
+  <si>
+    <t>28.05.20259</t>
+  </si>
+  <si>
+    <t>28.05.202510</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.066</v>
+        <v>0.082</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0.066</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>4.585</v>
+        <v>0.761</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>4.267</v>
+        <v>1.59</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>3.911</v>
+        <v>2.891</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>3.798</v>
+        <v>3.092</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>3.236</v>
+        <v>2.857</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>2.568</v>
+        <v>2.582</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>1.466</v>
+        <v>1.771</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0.539</v>
+        <v>0.892</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0.041</v>
+        <v>0.338</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>0.033</v>
+        <v>0.043</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45784</v>
+        <v>45798</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45785</v>
+        <v>45798</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C16">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>0.054</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>0.322</v>
+        <v>0.074</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>0.641</v>
+        <v>0.357</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>0.849</v>
+        <v>0.786</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0.979</v>
+        <v>1.283</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>1.053</v>
+        <v>1.788</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B28">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>1.855</v>
+        <v>2.408</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>2.796</v>
+        <v>2.576</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>2.401</v>
+        <v>2.58</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>2.042</v>
+        <v>3.054</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>1.683</v>
+        <v>3.198</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0.989</v>
+        <v>2.603</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0.597</v>
+        <v>1.913</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0.231</v>
+        <v>1.397</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>0.033</v>
+        <v>0.531</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B37">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>0.033</v>
+        <v>0.082</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45786</v>
+        <v>45799</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C40">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>0.8080000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>1.985</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>3.434</v>
+        <v>1.064</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>4.374</v>
+        <v>1.575</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>4.678</v>
+        <v>2.057</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>4.059</v>
+        <v>2.795</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>4.235</v>
+        <v>3.122</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>4.017</v>
+        <v>3.3</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>4.178</v>
+        <v>3.297</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>3.555</v>
+        <v>2.818</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>2.698</v>
+        <v>2.556</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>1.484</v>
+        <v>1.546</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0.5600000000000001</v>
+        <v>0.916</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0.051</v>
+        <v>0.539</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>0.033</v>
+        <v>0.075</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C62">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45786</v>
+        <v>45800</v>
       </c>
       <c r="B63">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C63">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45787</v>
+        <v>45800</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>0.239</v>
+        <v>0.169</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>0.379</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>0.777</v>
+        <v>1.754</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>1.074</v>
+        <v>2.733</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>1.686</v>
+        <v>3.181</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>2.055</v>
+        <v>3.617</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>2.384</v>
+        <v>3.822</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>2.296</v>
+        <v>3.841</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B79">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>2.081</v>
+        <v>3.652</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>1.789</v>
+        <v>3.355</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>1.256</v>
+        <v>2.436</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B82">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0.782</v>
+        <v>1.742</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C83">
-        <v>0.319</v>
+        <v>1.073</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>0.041</v>
+        <v>0.535</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B85">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85">
-        <v>0.033</v>
+        <v>0.076</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B86">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C86">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45787</v>
+        <v>45801</v>
       </c>
       <c r="B87">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C87">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45788</v>
+        <v>45801</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C88">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>0.083</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>0.665</v>
+        <v>0.104</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B96">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>1.502</v>
+        <v>0.413</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>2.127</v>
+        <v>0.747</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B98">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>2.971</v>
+        <v>1.091</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B99">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>3.493</v>
+        <v>1.522</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B100">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>3.948</v>
+        <v>1.583</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>4.06</v>
+        <v>1.995</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B102">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>3.934</v>
+        <v>2.454</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>3.657</v>
+        <v>2.277</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>2.951</v>
+        <v>1.786</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B105">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>2.02</v>
+        <v>1.461</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>1.392</v>
+        <v>1.136</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0.519</v>
+        <v>0.708</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C108">
-        <v>0.048</v>
+        <v>0.335</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B109">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C109">
-        <v>0.033</v>
+        <v>0.053</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B110">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C110">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45788</v>
+        <v>45802</v>
       </c>
       <c r="B111">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C111">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45789</v>
+        <v>45802</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C112">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>0.034</v>
+        <v>0.01</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>0.034</v>
+        <v>0.016</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B117">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>0.034</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B118">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B119">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0.8149999999999999</v>
+        <v>0.117</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>2.037</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>3.348</v>
+        <v>0.928</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>4.008</v>
+        <v>1.56</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>4.625</v>
+        <v>1.839</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B124">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>4.13</v>
+        <v>2.433</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>4.08</v>
+        <v>2.794</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>4.007</v>
+        <v>2.893</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B127">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>4.018</v>
+        <v>2.586</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B128">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>3.305</v>
+        <v>2.287</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>2.669</v>
+        <v>1.774</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B130">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>1.573</v>
+        <v>1.469</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0.595</v>
+        <v>0.805</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B132">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0.054</v>
+        <v>0.378</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B133">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C133">
-        <v>0.033</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B134">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C134">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45789</v>
+        <v>45803</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C135">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45790</v>
+        <v>45803</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C136">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B141">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>0.114</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B143">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>0.774</v>
+        <v>0.132</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B144">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>1.7</v>
+        <v>0.636</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B145">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>2.524</v>
+        <v>1.216</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>3.143</v>
+        <v>1.647</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B147">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>3.806</v>
+        <v>2.018</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B148">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>3.966</v>
+        <v>2.452</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>3.936</v>
+        <v>2.434</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B150">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>3.659</v>
+        <v>2.489</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>3.371</v>
+        <v>2.419</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B152">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>2.82</v>
+        <v>1.765</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B153">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>1.793</v>
+        <v>1.666</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B154">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C154">
-        <v>1.019</v>
+        <v>1.497</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B155">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0.428</v>
+        <v>0.852</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B156">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C156">
-        <v>0.048</v>
+        <v>0.406</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B157">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>0.033</v>
+        <v>0.078</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C158">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="B159">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C159">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45791</v>
+        <v>45804</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C160">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C161">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B163">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B165">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>0.033</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>0.056</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>0.361</v>
+        <v>0.129</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B168">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>0.955</v>
+        <v>0.637</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B169">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>1.762</v>
+        <v>1.232</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45791</v>
+        <v>45805</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>2.838</v>
+        <v>1.682</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>